<commit_message>
Updated onenote and excel sheet
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD7C8D4-A953-4F09-8012-95E2F749EFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C82FF9-5417-4378-B2E4-4038A7440212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -1891,10 +1891,10 @@
     <t>Very productive day. Satisfied with content</t>
   </si>
   <si>
-    <t>Woke up at 10:30 am, sat to study at 11am. Completed Normalisation PYQ. Started with Relational Algebra at 12:30pm</t>
-  </si>
-  <si>
-    <t>2hrs+</t>
+    <t>Woke up at 10:30 am, sat to study at 11am. Completed Normalisation PYQ. Started with Relational Algebra at 12:30pm. Did 25 Aptitude qs. Completed Relational Algebra revision</t>
+  </si>
+  <si>
+    <t>35qs, 50 pgs</t>
   </si>
 </sst>
 </file>
@@ -9900,10 +9900,10 @@
         <v>511</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>322</v>
+        <v>512</v>
       </c>
       <c r="E320" s="11" t="s">
-        <v>512</v>
+        <v>226</v>
       </c>
       <c r="F320" s="1" t="s">
         <v>352</v>

</xml_diff>

<commit_message>
Updated DBMS onenote, progress sheet
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEAD859-D841-491A-A6EF-0C0376CBE75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8CA1D9-895B-4BE8-9053-D57E03625B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="516">
   <si>
     <t>Date</t>
   </si>
@@ -1900,7 +1900,10 @@
     <t>Good day. Studied with heart full of content.</t>
   </si>
   <si>
-    <t xml:space="preserve">Woke up at 8:30am. Sat to study at 8:50 am. </t>
+    <t>Woke up at 8:30am. Sat to study at 8:50 am. Completed joins pyq.</t>
+  </si>
+  <si>
+    <t>2qs</t>
   </si>
 </sst>
 </file>
@@ -2715,7 +2718,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A314" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C321" sqref="C321"/>
+      <selection activeCell="E321" sqref="E321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9918,7 +9921,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="321" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" s="10">
         <v>44828</v>
       </c>
@@ -9928,8 +9931,11 @@
       <c r="C321" s="1" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="322" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D321" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A322" s="10">
         <v>44829</v>
       </c>
@@ -9937,7 +9943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="323" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="10">
         <v>44830</v>
       </c>
@@ -9945,7 +9951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="324" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" s="10">
         <v>44831</v>
       </c>
@@ -9953,7 +9959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="325" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A325" s="10">
         <v>44832</v>
       </c>
@@ -9961,7 +9967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="326" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A326" s="10">
         <v>44833</v>
       </c>
@@ -9969,7 +9975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="327" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A327" s="10">
         <v>44834</v>
       </c>
@@ -9977,7 +9983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="328" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A328" s="10">
         <v>44835</v>
       </c>
@@ -9985,7 +9991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="329" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A329" s="10">
         <v>44836</v>
       </c>
@@ -9993,7 +9999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="330" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A330" s="10">
         <v>44837</v>
       </c>
@@ -10001,7 +10007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="331" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A331" s="10">
         <v>44838</v>
       </c>
@@ -10009,7 +10015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="332" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A332" s="10">
         <v>44839</v>
       </c>
@@ -10017,7 +10023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="333" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A333" s="10">
         <v>44840</v>
       </c>
@@ -10025,7 +10031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="334" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A334" s="10">
         <v>44841</v>
       </c>
@@ -10033,7 +10039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="335" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A335" s="10">
         <v>44842</v>
       </c>
@@ -10041,7 +10047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="336" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A336" s="10">
         <v>44843</v>
       </c>

</xml_diff>

<commit_message>
Updated all the sheets
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CD2119-F22D-48B0-A608-8CCB46D1225C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA2CCFE-3369-45F0-AFB8-E9C9C4E5E536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1913" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="518">
   <si>
     <t>Date</t>
   </si>
@@ -1904,6 +1904,12 @@
   </si>
   <si>
     <t>Woke up at 8:30am. Sat to study at 8:50 am. Completed joins pyq. Completed Relational Algebra pyq</t>
+  </si>
+  <si>
+    <t>Woke up at 10 am. Mahalaya. Gave Unacademy Combat</t>
+  </si>
+  <si>
+    <t>25qs</t>
   </si>
 </sst>
 </file>
@@ -2717,8 +2723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A315" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C319" sqref="C319"/>
+    <sheetView tabSelected="1" topLeftCell="A316" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C320" sqref="C320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9950,6 +9956,21 @@
       </c>
       <c r="B322" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="E322" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="F322" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G322" s="12" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="323" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed Relational Calculus PYQ
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA2CCFE-3369-45F0-AFB8-E9C9C4E5E536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA5D6AC-B624-43F6-8903-B5E0CA73C7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="520">
   <si>
     <t>Date</t>
   </si>
@@ -1910,6 +1910,12 @@
   </si>
   <si>
     <t>25qs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Started studying qat 9 am. Completed Relational Calculus, safe query in 2hrs. </t>
+  </si>
+  <si>
+    <t>16qs</t>
   </si>
 </sst>
 </file>
@@ -2724,7 +2730,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A316" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C320" sqref="C320"/>
+      <selection activeCell="G323" sqref="G323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9979,6 +9985,18 @@
       </c>
       <c r="B323" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="E323" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F323" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="324" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated Apti and Excel sheets
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8CCFD6-73B6-40A4-B868-2A8EE20D5F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40442B82-BE40-4033-A465-AA0F9AA98D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="523">
   <si>
     <t>Date</t>
   </si>
@@ -1918,7 +1918,13 @@
     <t>16qs</t>
   </si>
   <si>
-    <t xml:space="preserve">Did aptitude till q 175 for 1.5 hrs. After  that wasted a lot of time behind an algo q. </t>
+    <t>Did aptitude till q 175 for 1.5 hrs. After  that wasted a lot of time behind an algo q.  Completed SQL revision. Did 21 SQL Pyqs.</t>
+  </si>
+  <si>
+    <t>21qs</t>
+  </si>
+  <si>
+    <t>Good Study. Could have studied more</t>
   </si>
 </sst>
 </file>
@@ -2733,7 +2739,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A317" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C321" sqref="C321"/>
+      <selection activeCell="D322" sqref="D322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10015,11 +10021,17 @@
       <c r="C324" s="1" t="s">
         <v>520</v>
       </c>
+      <c r="D324" s="1" t="s">
+        <v>521</v>
+      </c>
       <c r="E324" s="11" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="F324" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="G324" s="24" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="325" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated my progress and completed SQL
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AAD668-D27B-4C96-8604-4C09E3291F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E9B519-471A-43F6-A999-0784BA65BB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="527">
   <si>
     <t>Date</t>
   </si>
@@ -1927,10 +1927,16 @@
     <t>Good Study. Could have studied more</t>
   </si>
   <si>
-    <t>Woke up at 9am. Today is Tritiya. Completed all 51 SQL questions</t>
-  </si>
-  <si>
     <t>45qs</t>
+  </si>
+  <si>
+    <t>Woke up at 9am. Today is Tritiya. Completed all 51 SQL questions. Started revising Indexing, fIles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy with today's study. Good progress. </t>
+  </si>
+  <si>
+    <t>Woke up at 7:40 am. Started studying at 8:30am. Revising files : watched Sanchit Sir vids on indexing for numericals</t>
   </si>
 </sst>
 </file>
@@ -2745,7 +2751,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A321" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G325" sqref="G325"/>
+      <selection activeCell="E326" sqref="E326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10048,16 +10054,19 @@
         <v>10</v>
       </c>
       <c r="C325" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D325" s="11" t="s">
         <v>523</v>
       </c>
-      <c r="D325" s="11" t="s">
-        <v>524</v>
-      </c>
       <c r="E325" s="11" t="s">
-        <v>360</v>
+        <v>203</v>
       </c>
       <c r="F325" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="G325" s="13" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="326" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -10066,6 +10075,9 @@
       </c>
       <c r="B326" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="327" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated my current revision work
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EA6FD5-F70B-4185-9FC4-433267857149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3C9345-339F-4F46-B767-C353A67E80E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="544">
   <si>
     <t>Date</t>
   </si>
@@ -1979,6 +1979,15 @@
   </si>
   <si>
     <t>Good Study. Getting my form back :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woke up at 10:30 am. Started revising transaction management from 12pm. </t>
+  </si>
+  <si>
+    <t>16pgs</t>
+  </si>
+  <si>
+    <t>50m</t>
   </si>
 </sst>
 </file>
@@ -2803,7 +2812,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A328" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D332" sqref="D332"/>
+      <selection activeCell="G335" sqref="G335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10334,6 +10343,18 @@
       </c>
       <c r="B335" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="E335" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="F335" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="336" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed Trancn mgmt revision
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3C9345-339F-4F46-B767-C353A67E80E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827EE7E7-1A42-4735-A58D-94FBDF1AF577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="544">
   <si>
     <t>Date</t>
   </si>
@@ -1981,13 +1981,13 @@
     <t>Good Study. Getting my form back :)</t>
   </si>
   <si>
-    <t xml:space="preserve">Woke up at 10:30 am. Started revising transaction management from 12pm. </t>
-  </si>
-  <si>
-    <t>16pgs</t>
-  </si>
-  <si>
-    <t>50m</t>
+    <t>Woke up at 10:30 am. Started revising transaction management from 12pm. Completed transaction mgmt revision in 2.5 hrs.</t>
+  </si>
+  <si>
+    <t>43pgs</t>
+  </si>
+  <si>
+    <t>Good going till now :)</t>
   </si>
 </sst>
 </file>
@@ -10351,10 +10351,13 @@
         <v>542</v>
       </c>
       <c r="E335" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="F335" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G335" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="F335" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="336" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed conflict serizable pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827EE7E7-1A42-4735-A58D-94FBDF1AF577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0D75C9-6632-495E-BBC5-14F2777C4ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -1981,13 +1981,13 @@
     <t>Good Study. Getting my form back :)</t>
   </si>
   <si>
-    <t>Woke up at 10:30 am. Started revising transaction management from 12pm. Completed transaction mgmt revision in 2.5 hrs.</t>
-  </si>
-  <si>
     <t>43pgs</t>
   </si>
   <si>
     <t>Good going till now :)</t>
+  </si>
+  <si>
+    <t>Woke up at 10:30 am. Started revising transaction management from 12pm. Completed transaction mgmt revision in 2.5 hrs. Completed conflict serialzable pyqs.</t>
   </si>
 </sst>
 </file>
@@ -2812,7 +2812,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A328" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G335" sqref="G335"/>
+      <selection activeCell="F335" sqref="F335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10345,19 +10345,19 @@
         <v>6</v>
       </c>
       <c r="C335" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D335" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="D335" s="1" t="s">
+      <c r="E335" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F335" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G335" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="E335" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="F335" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="G335" s="1" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="336" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed Timestamp OP pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0D75C9-6632-495E-BBC5-14F2777C4ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6936A555-68D0-4C70-BFD0-63487E03D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -1987,7 +1987,7 @@
     <t>Good going till now :)</t>
   </si>
   <si>
-    <t>Woke up at 10:30 am. Started revising transaction management from 12pm. Completed transaction mgmt revision in 2.5 hrs. Completed conflict serialzable pyqs.</t>
+    <t>Woke up at 10:30 am. Started revising transaction management from 12pm. Completed transaction mgmt revision in 2.5 hrs. Completed conflict serialzable pyqs, TSO protocol pyqs</t>
   </si>
 </sst>
 </file>
@@ -2811,8 +2811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A328" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F335" sqref="F335"/>
+    <sheetView tabSelected="1" topLeftCell="A329" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D336" sqref="D336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10351,7 +10351,7 @@
         <v>541</v>
       </c>
       <c r="E335" s="11" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F335" s="1" t="s">
         <v>352</v>

</xml_diff>

<commit_message>
Updated 8th Oct 22
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6936A555-68D0-4C70-BFD0-63487E03D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCDAE9F-0CAB-4768-B227-21AB7730C458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -1984,10 +1984,10 @@
     <t>43pgs</t>
   </si>
   <si>
-    <t>Good going till now :)</t>
-  </si>
-  <si>
     <t>Woke up at 10:30 am. Started revising transaction management from 12pm. Completed transaction mgmt revision in 2.5 hrs. Completed conflict serialzable pyqs, TSO protocol pyqs</t>
+  </si>
+  <si>
+    <t>A very productive day after a long time :)</t>
   </si>
 </sst>
 </file>
@@ -2812,7 +2812,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A329" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D336" sqref="D336"/>
+      <selection activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10345,19 +10345,19 @@
         <v>6</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D335" s="1" t="s">
         <v>541</v>
       </c>
       <c r="E335" s="11" t="s">
-        <v>287</v>
+        <v>226</v>
       </c>
       <c r="F335" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G335" s="1" t="s">
-        <v>542</v>
+      <c r="G335" s="13" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="336" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
9th Oct 22 updates
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCDAE9F-0CAB-4768-B227-21AB7730C458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439C77F0-7AF4-41AD-9E88-F927D159FC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="545">
   <si>
     <t>Date</t>
   </si>
@@ -1988,6 +1988,9 @@
   </si>
   <si>
     <t>A very productive day after a long time :)</t>
+  </si>
+  <si>
+    <t>Sat to study at 1pm. Doing transaction pyqs</t>
   </si>
 </sst>
 </file>
@@ -2812,7 +2815,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A329" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C333" sqref="C333"/>
+      <selection activeCell="G336" sqref="G336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10366,6 +10369,15 @@
       </c>
       <c r="B336" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E336" s="11" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated 9th Oct 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB45B1D-935A-4D0B-B324-B3FA784B6491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B684C8B-A050-4B58-80D2-3ABA9FD705B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -1990,13 +1990,13 @@
     <t>A very productive day after a long time :)</t>
   </si>
   <si>
-    <t>Sat to study at 1pm. Doing transaction pyqs. Completed DBMS all Pyqs</t>
-  </si>
-  <si>
     <t>28qs</t>
   </si>
   <si>
-    <t>Great going.</t>
+    <t>Sat to study at 1pm. Doing transaction pyqs. Completed DBMS all Pyqs. Gave DBMS - 1 test. Rank 10/444</t>
+  </si>
+  <si>
+    <t>Great going.  Very Good Day. Got good marks in DBMS 1 test</t>
   </si>
 </sst>
 </file>
@@ -2820,8 +2820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A329" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G336" sqref="G336"/>
+    <sheetView tabSelected="1" topLeftCell="B330" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10377,10 +10377,10 @@
         <v>7</v>
       </c>
       <c r="C336" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D336" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="D336" s="1" t="s">
-        <v>545</v>
       </c>
       <c r="E336" s="11" t="s">
         <v>377</v>
@@ -10388,7 +10388,7 @@
       <c r="F336" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G336" s="1" t="s">
+      <c r="G336" s="13" t="s">
         <v>546</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Entry of 10th oct 22
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B684C8B-A050-4B58-80D2-3ABA9FD705B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EC9C1D-BBD0-4DD6-B6A6-EAF539C590CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1988" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="548">
   <si>
     <t>Date</t>
   </si>
@@ -1997,6 +1997,9 @@
   </si>
   <si>
     <t>Great going.  Very Good Day. Got good marks in DBMS 1 test</t>
+  </si>
+  <si>
+    <t>Woke up at 9am. Sat at 10:30 am. Analyzing test</t>
   </si>
 </sst>
 </file>
@@ -2821,7 +2824,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B330" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C333" sqref="C333"/>
+      <selection activeCell="D337" sqref="D337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10392,15 +10395,18 @@
         <v>546</v>
       </c>
     </row>
-    <row r="337" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A337" s="10">
         <v>44844</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="338" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C337" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A338" s="10">
         <v>44845</v>
       </c>
@@ -10408,7 +10414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A339" s="10">
         <v>44846</v>
       </c>
@@ -10416,7 +10422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="340" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A340" s="10">
         <v>44847</v>
       </c>
@@ -10424,7 +10430,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="341" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A341" s="10">
         <v>44848</v>
       </c>
@@ -10432,7 +10438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="342" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A342" s="10">
         <v>44849</v>
       </c>
@@ -10440,7 +10446,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="343" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A343" s="10">
         <v>44850</v>
       </c>
@@ -10448,7 +10454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A344" s="10">
         <v>44851</v>
       </c>
@@ -10456,7 +10462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A345" s="10">
         <v>44852</v>
       </c>
@@ -10464,7 +10470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="346" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A346" s="10">
         <v>44853</v>
       </c>
@@ -10472,7 +10478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="347" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A347" s="10">
         <v>44854</v>
       </c>
@@ -10480,7 +10486,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A348" s="10">
         <v>44855</v>
       </c>
@@ -10488,7 +10494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="349" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A349" s="10">
         <v>44856</v>
       </c>
@@ -10496,7 +10502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="350" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A350" s="10">
         <v>44857</v>
       </c>
@@ -10504,7 +10510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A351" s="10">
         <v>44858</v>
       </c>
@@ -10512,7 +10518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A352" s="10">
         <v>44859</v>
       </c>

</xml_diff>

<commit_message>
Updated Subs revised notebook
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EC9C1D-BBD0-4DD6-B6A6-EAF539C590CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D2D05A-D509-4E24-8B7E-5506F64AEAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="550">
   <si>
     <t>Date</t>
   </si>
@@ -1999,7 +1999,13 @@
     <t>Great going.  Very Good Day. Got good marks in DBMS 1 test</t>
   </si>
   <si>
-    <t>Woke up at 9am. Sat at 10:30 am. Analyzing test</t>
+    <t>Woke up at 9am. Sat at 10:30 am. Analyzing test. Gave DBMS -2 Test. Rank : 5/284</t>
+  </si>
+  <si>
+    <t>18qs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very good score. </t>
   </si>
 </sst>
 </file>
@@ -2823,8 +2829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B330" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D337" sqref="D337"/>
+    <sheetView tabSelected="1" topLeftCell="A314" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C319" sqref="C319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10389,13 +10395,13 @@
         <v>377</v>
       </c>
       <c r="F336" s="1" t="s">
-        <v>352</v>
+        <v>400</v>
       </c>
       <c r="G336" s="13" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="337" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A337" s="10">
         <v>44844</v>
       </c>
@@ -10405,8 +10411,20 @@
       <c r="C337" s="1" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="338" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D337" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="E337" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F337" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G337" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A338" s="10">
         <v>44845</v>
       </c>
@@ -10414,7 +10432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="339" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A339" s="10">
         <v>44846</v>
       </c>
@@ -10422,7 +10440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="340" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A340" s="10">
         <v>44847</v>
       </c>
@@ -10430,7 +10448,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="341" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A341" s="10">
         <v>44848</v>
       </c>
@@ -10438,7 +10456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="342" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A342" s="10">
         <v>44849</v>
       </c>
@@ -10446,7 +10464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="343" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A343" s="10">
         <v>44850</v>
       </c>
@@ -10454,7 +10472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="344" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A344" s="10">
         <v>44851</v>
       </c>
@@ -10462,7 +10480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="345" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A345" s="10">
         <v>44852</v>
       </c>
@@ -10470,7 +10488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="346" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A346" s="10">
         <v>44853</v>
       </c>
@@ -10478,7 +10496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="347" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A347" s="10">
         <v>44854</v>
       </c>
@@ -10486,7 +10504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="348" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A348" s="10">
         <v>44855</v>
       </c>
@@ -10494,7 +10512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="349" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A349" s="10">
         <v>44856</v>
       </c>
@@ -10502,7 +10520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="350" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A350" s="10">
         <v>44857</v>
       </c>
@@ -10510,7 +10528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="351" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A351" s="10">
         <v>44858</v>
       </c>
@@ -10518,7 +10536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="352" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A352" s="10">
         <v>44859</v>
       </c>

</xml_diff>

<commit_message>
Added 11th Oct 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE7D273-19DC-477F-9509-4C78FF0C716B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32BA849-3DA0-4F52-834A-61EB2CD2D433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="552">
   <si>
     <t>Date</t>
   </si>
@@ -2006,6 +2006,12 @@
   </si>
   <si>
     <t>Very good score. Next exam bad score :(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Started revising TOC. </t>
+  </si>
+  <si>
+    <t>28pgs</t>
   </si>
 </sst>
 </file>
@@ -2830,7 +2836,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A331" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G337" sqref="G337"/>
+      <selection activeCell="F338" sqref="F338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10430,6 +10436,15 @@
       </c>
       <c r="B338" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="E338" s="11" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="339" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updates to the sheet
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32BA849-3DA0-4F52-834A-61EB2CD2D433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361D7414-39C0-49F3-930F-ECE5328DFF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -2008,10 +2008,10 @@
     <t>Very good score. Next exam bad score :(</t>
   </si>
   <si>
-    <t xml:space="preserve">Started revising TOC. </t>
-  </si>
-  <si>
-    <t>28pgs</t>
+    <t>Started revising TOC. Completed Chp -0, Chp -1 : till Lec -4 done</t>
+  </si>
+  <si>
+    <t>56pgs till 282</t>
   </si>
 </sst>
 </file>
@@ -2836,7 +2836,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A331" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F338" sqref="F338"/>
+      <selection activeCell="D337" sqref="D337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10444,7 +10444,7 @@
         <v>551</v>
       </c>
       <c r="E338" s="11" t="s">
-        <v>394</v>
+        <v>277</v>
       </c>
     </row>
     <row r="339" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ToC completing fast :)
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361D7414-39C0-49F3-930F-ECE5328DFF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85041F2B-5011-46CC-89F7-7B712758941D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -2008,10 +2008,10 @@
     <t>Very good score. Next exam bad score :(</t>
   </si>
   <si>
-    <t>Started revising TOC. Completed Chp -0, Chp -1 : till Lec -4 done</t>
-  </si>
-  <si>
-    <t>56pgs till 282</t>
+    <t>Started revising TOC. Completed Chp -0, Chp -1 : till Lec -6 done</t>
+  </si>
+  <si>
+    <t>100 pgs till 323</t>
   </si>
 </sst>
 </file>
@@ -2835,8 +2835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A331" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D337" sqref="D337"/>
+    <sheetView tabSelected="1" topLeftCell="A332" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G338" sqref="G338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10444,7 +10444,7 @@
         <v>551</v>
       </c>
       <c r="E338" s="11" t="s">
-        <v>277</v>
+        <v>69</v>
       </c>
     </row>
     <row r="339" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated sheet with 12th Oct 22
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4396C9E-C4B8-4A3E-9C16-8BC5A1BB7C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62C590F-4770-4219-85B1-206CF46C30BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1999" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="555">
   <si>
     <t>Date</t>
   </si>
@@ -2011,13 +2011,16 @@
     <t>Started revising TOC. Completed Chp -0, Chp -1 : till Lec -6 done</t>
   </si>
   <si>
-    <t>100 pgs till 323</t>
-  </si>
-  <si>
     <t>4HR</t>
   </si>
   <si>
-    <t>Studying from 12;30PM</t>
+    <t>Studying from 12;30PM. Completed Lang to Machines, Machines -&gt; Regex</t>
+  </si>
+  <si>
+    <t>44 pgs till 344</t>
+  </si>
+  <si>
+    <t>100 pgs till 302</t>
   </si>
 </sst>
 </file>
@@ -2842,7 +2845,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A332" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C339" sqref="C339"/>
+      <selection activeCell="G339" sqref="G339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10447,10 +10450,10 @@
         <v>550</v>
       </c>
       <c r="D338" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="E338" s="11" t="s">
         <v>551</v>
-      </c>
-      <c r="E338" s="11" t="s">
-        <v>552</v>
       </c>
       <c r="F338" s="1" t="s">
         <v>352</v>
@@ -10467,7 +10470,16 @@
         <v>10</v>
       </c>
       <c r="C339" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D339" s="1" t="s">
         <v>553</v>
+      </c>
+      <c r="E339" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F339" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="340" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added 14th Oct 2022 entry
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD6222A-5E03-4F70-B803-2B8286925537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B39ED7-6068-4626-A6FC-C40BCA32B950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="561">
   <si>
     <t>Date</t>
   </si>
@@ -2024,6 +2024,21 @@
   </si>
   <si>
     <t>Studying from 12;30PM. Completed Lang to Machines, Machines -&gt; Regex. Did 40 Aptitude qs</t>
+  </si>
+  <si>
+    <t>Awesome Day after a long time. Completed TOC Chp 1 full revision</t>
+  </si>
+  <si>
+    <t>100pgs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8hrs </t>
+  </si>
+  <si>
+    <t>Great day. Realised the power of pomodoro effect :)</t>
+  </si>
+  <si>
+    <t>Woke up at 7:30 am. Completed all daily chores and began studying at 8:50am. TOC Pyqs Chp 1 started</t>
   </si>
 </sst>
 </file>
@@ -2847,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C338" sqref="C338"/>
+    <sheetView tabSelected="1" topLeftCell="A339" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D341" sqref="D341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10495,6 +10510,21 @@
       <c r="B340" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C340" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D340" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="E340" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="F340" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G340" s="13" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="341" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A341" s="10">
@@ -10502,6 +10532,9 @@
       </c>
       <c r="B341" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="342" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated 15th Oct, added 16th Oct 22
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B260C0A3-A8FF-43F0-A68A-699908620CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9778FD0-CBF1-40D1-A96E-49D238064B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="564">
   <si>
     <t>Date</t>
   </si>
@@ -2042,6 +2042,12 @@
   </si>
   <si>
     <t>6hhrs</t>
+  </si>
+  <si>
+    <t>Came back from Balurghat to Siliguri. Could not study</t>
+  </si>
+  <si>
+    <t>Sat to study at 10am.</t>
   </si>
 </sst>
 </file>
@@ -2866,7 +2872,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A339" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E346" sqref="E346"/>
+      <selection activeCell="D343" sqref="D343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10559,6 +10565,21 @@
       <c r="B342" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C342" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E342" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="F342" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G342" s="12" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="343" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A343" s="10">
@@ -10566,6 +10587,9 @@
       </c>
       <c r="B343" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="344" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Made plans for future
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E3D9CE-DAB2-464C-A01E-C115D39C3038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FB0554-1B50-403F-962B-279AA09C4846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="568">
   <si>
     <t>Date</t>
   </si>
@@ -2047,10 +2047,19 @@
     <t>Came back from Balurghat to Siliguri. Could not study</t>
   </si>
   <si>
-    <t>Sat to study at 10am. Completed FA qs by 2pm</t>
-  </si>
-  <si>
     <t>41qs</t>
+  </si>
+  <si>
+    <t>Sat to study at 10am. Completed FA qs by 2pm. Aptitude 30qs. TOC chp 2 revised except PDA prog.</t>
+  </si>
+  <si>
+    <t>Sat to study at 10 am. Planning for the left months.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES, I am BACK :)))) 10 hrs effectively studied. </t>
+  </si>
+  <si>
+    <t>NO STUDY. CAME BACK TO SILIGURI</t>
   </si>
 </sst>
 </file>
@@ -2875,7 +2884,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A339" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F343" sqref="F343"/>
+      <selection activeCell="E343" sqref="E343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10581,7 +10590,7 @@
         <v>352</v>
       </c>
       <c r="G342" s="12" t="s">
-        <v>376</v>
+        <v>567</v>
       </c>
     </row>
     <row r="343" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -10592,13 +10601,19 @@
         <v>7</v>
       </c>
       <c r="C343" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D343" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="D343" s="1" t="s">
-        <v>564</v>
-      </c>
       <c r="E343" s="11" t="s">
-        <v>292</v>
+        <v>202</v>
+      </c>
+      <c r="F343" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G343" s="13" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="344" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -10607,6 +10622,9 @@
       </c>
       <c r="B344" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="345" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated sheet. Added 18th Oct 22
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294B008A-83E5-48B0-8194-43F90E73047B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BEB569-86EB-401B-8EA6-0401E0B3EEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2030" uniqueCount="570">
   <si>
     <t>Date</t>
   </si>
@@ -2059,7 +2059,13 @@
     <t>NO STUDY. CAME BACK TO SILIGURI</t>
   </si>
   <si>
-    <t xml:space="preserve">Sat to study at 10 am. Planning for the left months. Completed revising Chp 2 of TOC </t>
+    <t>Studying from 10am. Doing TOC Pyqs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sat to study at 10 am. Planning for the left months. Completed revising Chp 2 of TOC . Completed chp 3 of TOC also. Did 30 apti qs at night. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great study. Very happy :) </t>
   </si>
 </sst>
 </file>
@@ -2884,7 +2890,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A339" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D345" sqref="D345"/>
+      <selection activeCell="C344" sqref="C344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10624,13 +10630,19 @@
         <v>8</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D344" s="1" t="s">
         <v>367</v>
       </c>
       <c r="E344" s="11" t="s">
-        <v>360</v>
+        <v>202</v>
+      </c>
+      <c r="F344" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G344" s="13" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="345" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -10639,6 +10651,12 @@
       </c>
       <c r="B345" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="E345" s="11" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="346" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated Sheet with TOC status
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BEB569-86EB-401B-8EA6-0401E0B3EEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AD5035-F009-4B5A-B042-C189E52DC6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2030" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="570">
   <si>
     <t>Date</t>
   </si>
@@ -2059,13 +2059,13 @@
     <t>NO STUDY. CAME BACK TO SILIGURI</t>
   </si>
   <si>
-    <t>Studying from 10am. Doing TOC Pyqs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sat to study at 10 am. Planning for the left months. Completed revising Chp 2 of TOC . Completed chp 3 of TOC also. Did 30 apti qs at night. </t>
   </si>
   <si>
     <t xml:space="preserve">Great study. Very happy :) </t>
+  </si>
+  <si>
+    <t>Studying from 10am. Doing TOC Pyqs. Completed CFG pyqs, countable uncountable pyqs</t>
   </si>
 </sst>
 </file>
@@ -2890,7 +2890,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A339" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C344" sqref="C344"/>
+      <selection activeCell="F345" sqref="F345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10630,7 +10630,7 @@
         <v>8</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D344" s="1" t="s">
         <v>367</v>
@@ -10642,7 +10642,7 @@
         <v>352</v>
       </c>
       <c r="G344" s="13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="345" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -10653,10 +10653,13 @@
         <v>9</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>567</v>
+        <v>569</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>496</v>
       </c>
       <c r="E345" s="11" t="s">
-        <v>394</v>
+        <v>230</v>
       </c>
     </row>
     <row r="346" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updates to TOC, added good links
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD243E10-2D61-4356-9261-89F2979A1D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B048C03-7C7F-4FBA-B40A-67AAD3739F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="575">
   <si>
     <t>Date</t>
   </si>
@@ -2077,7 +2077,10 @@
     <t>Very very Happy. Studied for 12 hrs :))))))))) YES :))))))</t>
   </si>
   <si>
-    <t>Completed Minimal state automata pyqs, non determinism</t>
+    <t>Completed Minimal state automata pyqs, non determinism, Np, PL, PDA pyqs, RE,REC pyqs</t>
+  </si>
+  <si>
+    <t>70qs</t>
   </si>
 </sst>
 </file>
@@ -2902,7 +2905,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A340" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C347" sqref="C347"/>
+      <selection activeCell="D343" sqref="D343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10691,10 +10694,13 @@
         <v>573</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>383</v>
+        <v>574</v>
       </c>
       <c r="E346" s="11" t="s">
-        <v>292</v>
+        <v>202</v>
+      </c>
+      <c r="F346" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="347" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Systematic updates on TOC
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B048C03-7C7F-4FBA-B40A-67AAD3739F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C174DF64-39C8-4D64-9CEF-C2B5D9120F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2077,10 +2077,10 @@
     <t>Very very Happy. Studied for 12 hrs :))))))))) YES :))))))</t>
   </si>
   <si>
-    <t>Completed Minimal state automata pyqs, non determinism, Np, PL, PDA pyqs, RE,REC pyqs</t>
-  </si>
-  <si>
-    <t>70qs</t>
+    <t>Completed Minimal state automata pyqs, non determinism, Np, PL, PDA pyqs, RE,REC pyqs, reg exp qs</t>
+  </si>
+  <si>
+    <t>11hrs</t>
   </si>
 </sst>
 </file>
@@ -2904,8 +2904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D343" sqref="D343"/>
+    <sheetView tabSelected="1" topLeftCell="D343" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G346" sqref="G346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10694,10 +10694,10 @@
         <v>573</v>
       </c>
       <c r="D346" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E346" s="11" t="s">
         <v>574</v>
-      </c>
-      <c r="E346" s="11" t="s">
-        <v>202</v>
       </c>
       <c r="F346" s="1" t="s">
         <v>352</v>

</xml_diff>

<commit_message>
COMPLETED ALL TOC PYQS.
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C174DF64-39C8-4D64-9CEF-C2B5D9120F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4075DF-7A58-4F56-A63E-15B50BD7EF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="577">
   <si>
     <t>Date</t>
   </si>
@@ -2077,10 +2077,16 @@
     <t>Very very Happy. Studied for 12 hrs :))))))))) YES :))))))</t>
   </si>
   <si>
-    <t>Completed Minimal state automata pyqs, non determinism, Np, PL, PDA pyqs, RE,REC pyqs, reg exp qs</t>
-  </si>
-  <si>
-    <t>11hrs</t>
+    <t>Completed Minimal state automata pyqs, non determinism, Np, PL, PDA pyqs, RE,REC pyqs, reg exp qs. COMPLETED ALL TOC PYQs</t>
+  </si>
+  <si>
+    <t>16hrs</t>
+  </si>
+  <si>
+    <t>16HRS STUDIED. STILL FRESH :))))))))))))))</t>
+  </si>
+  <si>
+    <t>163qs</t>
   </si>
 </sst>
 </file>
@@ -2904,8 +2910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D343" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G346" sqref="G346"/>
+    <sheetView tabSelected="1" topLeftCell="A343" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E348" sqref="E348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10694,13 +10700,16 @@
         <v>573</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>469</v>
+        <v>576</v>
       </c>
       <c r="E346" s="11" t="s">
         <v>574</v>
       </c>
       <c r="F346" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="G346" s="13" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="347" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added TOC subject test progress
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E93E3A-6B39-44A7-BD24-7D6388A28BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9847DAE-DBB3-47EE-97E6-28F4EDF49444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="579">
   <si>
     <t>Date</t>
   </si>
@@ -2089,13 +2089,10 @@
     <t>163qs</t>
   </si>
   <si>
-    <t>Gave TOC topic tests - 1,2. Good Marks. Very confident in TOC</t>
-  </si>
-  <si>
-    <t>34qs</t>
-  </si>
-  <si>
-    <t>1.5hrs</t>
+    <t xml:space="preserve">Gave TOC topic tests - 1,2. Good Marks. Very confident in TOC. Secured 43/50 in TOC Subject test. RANK = 2 </t>
+  </si>
+  <si>
+    <t>70qs</t>
   </si>
 </sst>
 </file>
@@ -10735,7 +10732,7 @@
         <v>578</v>
       </c>
       <c r="E347" s="11" t="s">
-        <v>579</v>
+        <v>292</v>
       </c>
       <c r="F347" s="1" t="s">
         <v>400</v>

</xml_diff>

<commit_message>
Full TOC Completed :)
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9847DAE-DBB3-47EE-97E6-28F4EDF49444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A623D082-5621-4EB9-BBA8-804DD2B4C52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -2089,10 +2089,10 @@
     <t>163qs</t>
   </si>
   <si>
-    <t xml:space="preserve">Gave TOC topic tests - 1,2. Good Marks. Very confident in TOC. Secured 43/50 in TOC Subject test. RANK = 2 </t>
-  </si>
-  <si>
     <t>70qs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gave TOC topic tests - 1,2. Good Marks. Very confident in TOC. Secured 43/50 in TOC Subject test. RANK = 2. Fully completed TOC, including all TOC test analyses </t>
   </si>
 </sst>
 </file>
@@ -10726,13 +10726,13 @@
         <v>11</v>
       </c>
       <c r="C347" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D347" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="D347" s="1" t="s">
-        <v>578</v>
-      </c>
       <c r="E347" s="11" t="s">
-        <v>292</v>
+        <v>226</v>
       </c>
       <c r="F347" s="1" t="s">
         <v>400</v>

</xml_diff>

<commit_message>
Updated my excel sheet
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A623D082-5621-4EB9-BBA8-804DD2B4C52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FFC4F4-DE17-4F1C-AFE1-14A54A78CD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="583">
   <si>
     <t>Date</t>
   </si>
@@ -2093,6 +2093,18 @@
   </si>
   <si>
     <t xml:space="preserve">Gave TOC topic tests - 1,2. Good Marks. Very confident in TOC. Secured 43/50 in TOC Subject test. RANK = 2. Fully completed TOC, including all TOC test analyses </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 hrs studied. Gave the tests. Happy </t>
+  </si>
+  <si>
+    <t>Felt very tired the entire day. At evening, my friend had visited. No study the whole day</t>
+  </si>
+  <si>
+    <t>Couldn't study the entire day. Bad day</t>
+  </si>
+  <si>
+    <t>Sat to study ar 9: 50am. Started with C programming &amp; DS</t>
   </si>
 </sst>
 </file>
@@ -2917,7 +2929,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A343" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G347" sqref="G347"/>
+      <selection activeCell="D349" sqref="D349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10737,6 +10749,9 @@
       <c r="F347" s="1" t="s">
         <v>400</v>
       </c>
+      <c r="G347" s="13" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="348" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A348" s="10">
@@ -10745,6 +10760,21 @@
       <c r="B348" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C348" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E348" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="F348" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G348" s="12" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="349" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A349" s="10">
@@ -10752,6 +10782,9 @@
       </c>
       <c r="B349" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="350" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
22nd Oct 22, 1-5hrs done
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4535C3-54FA-4010-8B19-9F9F06F1C797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E26D162-454F-4971-99A8-21CE4920ABF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="583">
   <si>
     <t>Date</t>
   </si>
@@ -2104,10 +2104,7 @@
     <t>Couldn't study the entire day. Bad day</t>
   </si>
   <si>
-    <t>Sat to study ar 9: 50am. Started with C programming &amp; DS. Completed revising basics, types, operators, flow control, functions</t>
-  </si>
-  <si>
-    <t>26pgs</t>
+    <t>Sat to study ar 9: 50am. Started with C programming &amp; DS. Completed revising basics, types, operators, flow control, functions, scopes</t>
   </si>
 </sst>
 </file>
@@ -10790,10 +10787,10 @@
         <v>582</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>583</v>
+        <v>365</v>
       </c>
       <c r="E349" s="11" t="s">
-        <v>394</v>
+        <v>427</v>
       </c>
       <c r="F349" s="1" t="s">
         <v>352</v>

</xml_diff>

<commit_message>
Updated my sheet with my progress
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C83C39F-6225-4C6B-B24F-1E51634C4B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49318E11-5A69-48F0-8325-18825C37865A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="587">
   <si>
     <t>Date</t>
   </si>
@@ -2108,6 +2108,15 @@
   </si>
   <si>
     <t>51pgs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gave Full Syllabus Test -3. Scored : 62.7. Rank - 4. It was a really good q paper. Analysed it in a great way. </t>
+  </si>
+  <si>
+    <t>Good Day. At night there was a party at home.</t>
+  </si>
+  <si>
+    <t>Nice progress in C.</t>
   </si>
 </sst>
 </file>
@@ -2931,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A343" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E349" sqref="E349"/>
+    <sheetView tabSelected="1" topLeftCell="A344" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E351" sqref="E351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10793,10 +10802,13 @@
         <v>583</v>
       </c>
       <c r="E349" s="11" t="s">
-        <v>292</v>
+        <v>360</v>
       </c>
       <c r="F349" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="G349" s="13" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="350" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -10805,6 +10817,21 @@
       </c>
       <c r="B350" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E350" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F350" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G350" s="13" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="351" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added 24th Oct 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49318E11-5A69-48F0-8325-18825C37865A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22D54D-F134-4A58-B94B-04647361F234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="589">
   <si>
     <t>Date</t>
   </si>
@@ -2117,6 +2117,12 @@
   </si>
   <si>
     <t>Nice progress in C.</t>
+  </si>
+  <si>
+    <t>Today is Kali Puja. Completed revinsing C programming notes.</t>
+  </si>
+  <si>
+    <t>Very Little Study. At night went out for Pandal hopping</t>
   </si>
 </sst>
 </file>
@@ -2940,8 +2946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A344" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E351" sqref="E351"/>
+    <sheetView tabSelected="1" topLeftCell="A347" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C352" sqref="C352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10840,6 +10846,21 @@
       </c>
       <c r="B351" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E351" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F351" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G351" s="24" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="352" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added 25th Oct 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22D54D-F134-4A58-B94B-04647361F234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B55A93-6E55-4AB1-8B24-0F321E86BA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="590">
   <si>
     <t>Date</t>
   </si>
@@ -2123,6 +2123,9 @@
   </si>
   <si>
     <t>Very Little Study. At night went out for Pandal hopping</t>
+  </si>
+  <si>
+    <t>Started with C programming qs</t>
   </si>
 </sst>
 </file>
@@ -2947,7 +2950,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A347" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C352" sqref="C352"/>
+      <selection activeCell="E352" sqref="E352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10869,6 +10872,9 @@
       </c>
       <c r="B352" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed till Goto Function
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B55A93-6E55-4AB1-8B24-0F321E86BA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819375A1-2B7C-444B-A022-16EFD1C857E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2068" uniqueCount="591">
   <si>
     <t>Date</t>
   </si>
@@ -2125,7 +2125,10 @@
     <t>Very Little Study. At night went out for Pandal hopping</t>
   </si>
   <si>
-    <t>Started with C programming qs</t>
+    <t>Started with C programming qs. Completed till Goto fns</t>
+  </si>
+  <si>
+    <t>Littile study in the morning. Celebrated Diwali with Family Like a  KING!</t>
   </si>
 </sst>
 </file>
@@ -2950,7 +2953,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A347" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E352" sqref="E352"/>
+      <selection activeCell="C351" sqref="C351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10875,6 +10878,18 @@
       </c>
       <c r="C352" s="1" t="s">
         <v>589</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E352" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F352" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G352" s="24" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed till parameter passing
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819375A1-2B7C-444B-A022-16EFD1C857E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C98D4EB-4C15-48FC-B539-2E5846D487DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2068" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="593">
   <si>
     <t>Date</t>
   </si>
@@ -2129,6 +2129,12 @@
   </si>
   <si>
     <t>Littile study in the morning. Celebrated Diwali with Family Like a  KING!</t>
+  </si>
+  <si>
+    <t>Doing C programming pyqs. Going great. Completed upto parameter passing</t>
+  </si>
+  <si>
+    <t>24qs</t>
   </si>
 </sst>
 </file>
@@ -2953,7 +2959,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A347" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C351" sqref="C351"/>
+      <selection activeCell="F353" sqref="F353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10892,15 +10898,27 @@
         <v>590</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A353" s="10">
         <v>44860</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="354" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C353" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="E353" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F353" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A354" s="10">
         <v>44861</v>
       </c>
@@ -10908,7 +10926,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="355" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A355" s="10">
         <v>44862</v>
       </c>
@@ -10916,7 +10934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="356" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A356" s="10">
         <v>44863</v>
       </c>
@@ -10924,7 +10942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="357" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A357" s="10">
         <v>44864</v>
       </c>
@@ -10932,7 +10950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="358" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A358" s="10">
         <v>44865</v>
       </c>
@@ -10940,7 +10958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="359" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A359" s="10">
         <v>44866</v>
       </c>
@@ -10948,7 +10966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="360" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A360" s="10">
         <v>44867</v>
       </c>
@@ -10956,7 +10974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A361" s="10">
         <v>44868</v>
       </c>
@@ -10964,7 +10982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="362" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A362" s="10">
         <v>44869</v>
       </c>
@@ -10972,7 +10990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="363" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A363" s="10">
         <v>44870</v>
       </c>
@@ -10980,7 +10998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="364" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A364" s="10">
         <v>44871</v>
       </c>
@@ -10988,7 +11006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="365" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A365" s="10">
         <v>44872</v>
       </c>
@@ -10996,7 +11014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A366" s="10">
         <v>44873</v>
       </c>
@@ -11004,7 +11022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A367" s="10">
         <v>44874</v>
       </c>
@@ -11012,7 +11030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="368" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A368" s="10">
         <v>44875</v>
       </c>

</xml_diff>

<commit_message>
Added 27th Oct 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C98D4EB-4C15-48FC-B539-2E5846D487DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B374C72-F4BF-4D86-A956-4A39EC0263A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="594">
   <si>
     <t>Date</t>
   </si>
@@ -2134,7 +2134,10 @@
     <t>Doing C programming pyqs. Going great. Completed upto parameter passing</t>
   </si>
   <si>
-    <t>24qs</t>
+    <t>Good Study. Learnt many new C Prog concepts</t>
+  </si>
+  <si>
+    <t>Started studying at 10:30am. Today is Bhai Phota</t>
   </si>
 </sst>
 </file>
@@ -2959,7 +2962,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A347" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F353" sqref="F353"/>
+      <selection activeCell="D354" sqref="D354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10898,7 +10901,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="353" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A353" s="10">
         <v>44860</v>
       </c>
@@ -10909,24 +10912,30 @@
         <v>591</v>
       </c>
       <c r="D353" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E353" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="F353" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G353" s="13" t="s">
         <v>592</v>
       </c>
-      <c r="E353" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="F353" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="354" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="354" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A354" s="10">
         <v>44861</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="355" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C354" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A355" s="10">
         <v>44862</v>
       </c>
@@ -10934,7 +10943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="356" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A356" s="10">
         <v>44863</v>
       </c>
@@ -10942,7 +10951,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="357" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A357" s="10">
         <v>44864</v>
       </c>
@@ -10950,7 +10959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="358" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A358" s="10">
         <v>44865</v>
       </c>
@@ -10958,7 +10967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="359" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A359" s="10">
         <v>44866</v>
       </c>
@@ -10966,7 +10975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="360" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A360" s="10">
         <v>44867</v>
       </c>
@@ -10974,7 +10983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="361" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A361" s="10">
         <v>44868</v>
       </c>
@@ -10982,7 +10991,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="362" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A362" s="10">
         <v>44869</v>
       </c>
@@ -10990,7 +10999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="363" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A363" s="10">
         <v>44870</v>
       </c>
@@ -10998,7 +11007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="364" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A364" s="10">
         <v>44871</v>
       </c>
@@ -11006,7 +11015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="365" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A365" s="10">
         <v>44872</v>
       </c>
@@ -11014,7 +11023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="366" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A366" s="10">
         <v>44873</v>
       </c>
@@ -11022,7 +11031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="367" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A367" s="10">
         <v>44874</v>
       </c>
@@ -11030,7 +11039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="368" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A368" s="10">
         <v>44875</v>
       </c>

</xml_diff>

<commit_message>
Completed upto Programming paradigms
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD83EBA4-BA86-4C0B-AD83-9CAEF46FA086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13DACCF-95A8-413C-B4AE-DEB9531301CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="596">
   <si>
     <t>Date</t>
   </si>
@@ -2137,10 +2137,13 @@
     <t>Good Study. Learnt many new C Prog concepts</t>
   </si>
   <si>
-    <t>Started studying at 10:30am. Today is Bhai Phota. Did 12qs on C prog</t>
-  </si>
-  <si>
-    <t>12qs</t>
+    <t>Started studying at 10:30am. Today is Bhai Phota. Did 12qs on C prog. Completed upto programming paradigms</t>
+  </si>
+  <si>
+    <t>48qs</t>
+  </si>
+  <si>
+    <t>Good Study. Bhai phota in the morning</t>
   </si>
 </sst>
 </file>
@@ -2964,8 +2967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A347" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G354" sqref="G354"/>
+    <sheetView tabSelected="1" topLeftCell="B347" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C349" sqref="C349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10941,10 +10944,13 @@
         <v>594</v>
       </c>
       <c r="E354" s="11" t="s">
-        <v>427</v>
+        <v>360</v>
       </c>
       <c r="F354" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="G354" s="13" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="355" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed all C programming pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13DACCF-95A8-413C-B4AE-DEB9531301CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5248DD0-2128-4505-9FE7-4F1D904A85A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="597">
   <si>
     <t>Date</t>
   </si>
@@ -2144,6 +2144,9 @@
   </si>
   <si>
     <t>Good Study. Bhai phota in the morning</t>
+  </si>
+  <si>
+    <t>Completed all C programming pyqs</t>
   </si>
 </sst>
 </file>
@@ -2967,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B347" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C349" sqref="C349"/>
+    <sheetView tabSelected="1" topLeftCell="B348" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G355" sqref="G355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10959,6 +10962,18 @@
       </c>
       <c r="B355" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E355" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F355" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="356" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed linked List pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FA1AF8-5797-4990-8B24-CFAB4953E0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D293701-8031-45C9-AAC2-6E323DC792E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="601">
   <si>
     <t>Date</t>
   </si>
@@ -2152,13 +2152,13 @@
     <t>Day spent well. Did many Pyqs. But I can see that my efficiency has decreased.</t>
   </si>
   <si>
-    <t>1hr done</t>
-  </si>
-  <si>
-    <t>Studying since 10am. Started revising Data Structure.</t>
-  </si>
-  <si>
-    <t>13pgs</t>
+    <t>Studying since 10am. Started revising Data Structure. Completed LL along with pyqs</t>
+  </si>
+  <si>
+    <t>29pgs</t>
+  </si>
+  <si>
+    <t>Moderate day. Slow progress</t>
   </si>
 </sst>
 </file>
@@ -2982,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A349" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G356" sqref="G356"/>
+    <sheetView tabSelected="1" topLeftCell="B350" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D352" sqref="D352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10999,16 +10999,19 @@
         <v>6</v>
       </c>
       <c r="C356" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D356" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="D356" s="1" t="s">
+      <c r="E356" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="F356" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G356" s="24" t="s">
         <v>600</v>
-      </c>
-      <c r="E356" s="11" t="s">
-        <v>598</v>
-      </c>
-      <c r="F356" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="357" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed upto Queue Pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D293701-8031-45C9-AAC2-6E323DC792E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0FB774-D59F-4EB2-B7FB-0C131522129E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="602">
   <si>
     <t>Date</t>
   </si>
@@ -2159,6 +2159,9 @@
   </si>
   <si>
     <t>Moderate day. Slow progress</t>
+  </si>
+  <si>
+    <t>Completed Stacks , Queues revision also. Completed infix, postfix pyqs, queue pyqs</t>
   </si>
 </sst>
 </file>
@@ -2982,8 +2985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B350" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D352" sqref="D352"/>
+    <sheetView tabSelected="1" topLeftCell="A350" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G357" sqref="G357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11020,6 +11023,18 @@
       </c>
       <c r="B357" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E357" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="F357" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="358" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Did some minor changes in Gate planning
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2999D7FE-DA89-4D46-B81F-85166CA48E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF489895-3232-41C9-AC26-04A41D3A3589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="613">
   <si>
     <t>Date</t>
   </si>
@@ -2180,6 +2180,21 @@
   </si>
   <si>
     <t>Less study. Coimpleted DS pyq till AVL tree.</t>
+  </si>
+  <si>
+    <t>Busy with Project. Did some qs of BST</t>
+  </si>
+  <si>
+    <t>Less study.</t>
+  </si>
+  <si>
+    <t>Project submission. At night studied for 2 hrs</t>
+  </si>
+  <si>
+    <t>Did BST pyqs. Less study</t>
+  </si>
+  <si>
+    <t>Completed BST qs</t>
   </si>
 </sst>
 </file>
@@ -3003,8 +3018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D361" sqref="D361"/>
+    <sheetView tabSelected="1" topLeftCell="A356" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G363" sqref="G363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11134,6 +11149,21 @@
       <c r="B361" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C361" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E361" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F361" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G361" s="24" t="s">
+        <v>609</v>
+      </c>
     </row>
     <row r="362" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A362" s="10">
@@ -11142,6 +11172,21 @@
       <c r="B362" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C362" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E362" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F362" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G362" s="24" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="363" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A363" s="10">
@@ -11149,6 +11194,15 @@
       </c>
       <c r="B363" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F363" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="364" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated 5th Nov 22
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF489895-3232-41C9-AC26-04A41D3A3589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F011C7-6AD3-4ECF-97DB-5B73E3AEB4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="615">
   <si>
     <t>Date</t>
   </si>
@@ -2194,7 +2194,13 @@
     <t>Did BST pyqs. Less study</t>
   </si>
   <si>
-    <t>Completed BST qs</t>
+    <t>Completed BST qs. Completed Binary Tree qs</t>
+  </si>
+  <si>
+    <t>61qs</t>
+  </si>
+  <si>
+    <t>Good study.</t>
   </si>
 </sst>
 </file>
@@ -3018,8 +3024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A356" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G363" sqref="G363"/>
+    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D365" sqref="D365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11199,10 +11205,16 @@
         <v>612</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>322</v>
+        <v>613</v>
+      </c>
+      <c r="E363" s="11" t="s">
+        <v>360</v>
       </c>
       <c r="F363" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="G363" s="13" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="364" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added 6th Nov 22
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F011C7-6AD3-4ECF-97DB-5B73E3AEB4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC25FA5-6CAD-40D0-B437-C30839361937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="616">
   <si>
     <t>Date</t>
   </si>
@@ -2201,6 +2201,9 @@
   </si>
   <si>
     <t>Good study.</t>
+  </si>
+  <si>
+    <t>Gave FST -4 of Made easy. Marks = 66.36</t>
   </si>
 </sst>
 </file>
@@ -3025,7 +3028,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A357" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D365" sqref="D365"/>
+      <selection activeCell="G364" sqref="G364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11223,6 +11226,18 @@
       </c>
       <c r="B364" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E364" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="F364" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="365" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated my eexcel sheet
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC25FA5-6CAD-40D0-B437-C30839361937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146328E9-D960-44D3-ADB2-20AD91C1F141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="623">
   <si>
     <t>Date</t>
   </si>
@@ -2203,7 +2203,28 @@
     <t>Good study.</t>
   </si>
   <si>
-    <t>Gave FST -4 of Made easy. Marks = 66.36</t>
+    <t>Gave FST -4 of Made easy. Marks = 66.36. Went out in evening</t>
+  </si>
+  <si>
+    <t>Gave Go classes test 1 on c prog. 18/35 marks. Analyzed the test fully.</t>
+  </si>
+  <si>
+    <t>Clg test in morning, went out in the evening. No study</t>
+  </si>
+  <si>
+    <t>Bad day. Declining performance</t>
+  </si>
+  <si>
+    <t>Completed graphs of DS</t>
+  </si>
+  <si>
+    <t>Little study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little study. Couldn’t do as planned </t>
+  </si>
+  <si>
+    <t>Gave  GO classes test 2 on c prog. 25/40 marks</t>
   </si>
 </sst>
 </file>
@@ -3027,8 +3048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G364" sqref="G364"/>
+    <sheetView tabSelected="1" topLeftCell="A365" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F369" sqref="F369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11239,6 +11260,9 @@
       <c r="F364" s="1" t="s">
         <v>400</v>
       </c>
+      <c r="G364" s="24" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="365" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A365" s="10">
@@ -11247,6 +11271,21 @@
       <c r="B365" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C365" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E365" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F365" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G365" s="24" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="366" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A366" s="10">
@@ -11255,6 +11294,21 @@
       <c r="B366" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C366" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="E366" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="F366" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G366" s="13" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="367" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A367" s="10">
@@ -11263,6 +11317,21 @@
       <c r="B367" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C367" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E367" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="F367" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G367" s="1" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="368" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A368" s="10">
@@ -11271,16 +11340,43 @@
       <c r="B368" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="369" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C368" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="D368" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E368" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="F368" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G368" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A369" s="10">
         <v>44876</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="370" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C369" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="D369" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E369" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="F369" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A370" s="10">
         <v>44877</v>
       </c>
@@ -11288,7 +11384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A371" s="10">
         <v>44878</v>
       </c>
@@ -11296,7 +11392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A372" s="10">
         <v>44879</v>
       </c>
@@ -11304,7 +11400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="373" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A373" s="10">
         <v>44880</v>
       </c>
@@ -11312,7 +11408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A374" s="10">
         <v>44881</v>
       </c>
@@ -11320,7 +11416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A375" s="10">
         <v>44882</v>
       </c>
@@ -11328,7 +11424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A376" s="10">
         <v>44883</v>
       </c>
@@ -11336,7 +11432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="377" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A377" s="10">
         <v>44884</v>
       </c>
@@ -11344,7 +11440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="378" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A378" s="10">
         <v>44885</v>
       </c>
@@ -11352,7 +11448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="379" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A379" s="10">
         <v>44886</v>
       </c>
@@ -11360,7 +11456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="380" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A380" s="10">
         <v>44887</v>
       </c>
@@ -11368,7 +11464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="381" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A381" s="10">
         <v>44888</v>
       </c>
@@ -11376,7 +11472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="382" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A382" s="10">
         <v>44889</v>
       </c>
@@ -11384,7 +11480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A383" s="10">
         <v>44890</v>
       </c>
@@ -11392,7 +11488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="384" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A384" s="10">
         <v>44891</v>
       </c>

</xml_diff>

<commit_message>
Added 12th Nov 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146328E9-D960-44D3-ADB2-20AD91C1F141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F4090F-330F-417D-8A2D-5A19CA8F7956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="626">
   <si>
     <t>Date</t>
   </si>
@@ -2224,7 +2224,16 @@
     <t xml:space="preserve">Little study. Couldn’t do as planned </t>
   </si>
   <si>
-    <t>Gave  GO classes test 2 on c prog. 25/40 marks</t>
+    <t>Gave  GO classes test 2 on c prog. 25/40 marks. Analyzed full test</t>
+  </si>
+  <si>
+    <t>Very Good Study.</t>
+  </si>
+  <si>
+    <t>Completed DS full revision ans well as PYQs</t>
+  </si>
+  <si>
+    <t>40pgs &amp; 16qs</t>
   </si>
 </sst>
 </file>
@@ -3048,8 +3057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A365" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F369" sqref="F369"/>
+    <sheetView tabSelected="1" topLeftCell="B365" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G370" sqref="G370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11329,7 +11338,7 @@
       <c r="F367" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G367" s="1" t="s">
+      <c r="G367" s="12" t="s">
         <v>618</v>
       </c>
     </row>
@@ -11352,11 +11361,11 @@
       <c r="F368" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G368" s="1" t="s">
+      <c r="G368" s="12" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="369" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A369" s="10">
         <v>44876</v>
       </c>
@@ -11370,21 +11379,36 @@
         <v>544</v>
       </c>
       <c r="E369" s="11" t="s">
-        <v>277</v>
+        <v>226</v>
       </c>
       <c r="F369" s="1" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="370" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G369" s="13" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A370" s="10">
         <v>44877</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="371" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C370" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="D370" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="E370" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="F370" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A371" s="10">
         <v>44878</v>
       </c>
@@ -11392,7 +11416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="372" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A372" s="10">
         <v>44879</v>
       </c>
@@ -11400,7 +11424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A373" s="10">
         <v>44880</v>
       </c>
@@ -11408,7 +11432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="374" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A374" s="10">
         <v>44881</v>
       </c>
@@ -11416,7 +11440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="375" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A375" s="10">
         <v>44882</v>
       </c>
@@ -11424,7 +11448,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="376" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A376" s="10">
         <v>44883</v>
       </c>
@@ -11432,7 +11456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="377" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A377" s="10">
         <v>44884</v>
       </c>
@@ -11440,7 +11464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="378" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A378" s="10">
         <v>44885</v>
       </c>
@@ -11448,7 +11472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="379" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A379" s="10">
         <v>44886</v>
       </c>
@@ -11456,7 +11480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="380" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A380" s="10">
         <v>44887</v>
       </c>
@@ -11464,7 +11488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="381" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A381" s="10">
         <v>44888</v>
       </c>
@@ -11472,7 +11496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="382" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A382" s="10">
         <v>44889</v>
       </c>
@@ -11480,7 +11504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="383" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A383" s="10">
         <v>44890</v>
       </c>
@@ -11488,7 +11512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="384" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A384" s="10">
         <v>44891</v>
       </c>

</xml_diff>

<commit_message>
Updated 12th Nov 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F4090F-330F-417D-8A2D-5A19CA8F7956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55CFE98-5474-423C-B420-D65ECF6414A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="628">
   <si>
     <t>Date</t>
   </si>
@@ -2230,10 +2230,16 @@
     <t>Very Good Study.</t>
   </si>
   <si>
-    <t>Completed DS full revision ans well as PYQs</t>
-  </si>
-  <si>
-    <t>40pgs &amp; 16qs</t>
+    <t>Completed DS full revision ans well as PYQs. Gave Go test on Hashing, analyzed also</t>
+  </si>
+  <si>
+    <t>40pgs &amp; 40qs</t>
+  </si>
+  <si>
+    <t>11hrs</t>
+  </si>
+  <si>
+    <t>Very very Happy. Studied for 11 hrs :))))))))) YES :))))))</t>
   </si>
 </sst>
 </file>
@@ -3058,7 +3064,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B365" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G370" sqref="G370"/>
+      <selection activeCell="C369" sqref="C369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11402,10 +11408,13 @@
         <v>625</v>
       </c>
       <c r="E370" s="11" t="s">
-        <v>287</v>
+        <v>626</v>
       </c>
       <c r="F370" s="1" t="s">
-        <v>352</v>
+        <v>400</v>
+      </c>
+      <c r="G370" s="33" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="371" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated 13th Nov 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55CFE98-5474-423C-B420-D65ECF6414A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0599FF8-206F-4C34-8AFA-35969CB7085E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="630">
   <si>
     <t>Date</t>
   </si>
@@ -2240,6 +2240,12 @@
   </si>
   <si>
     <t>Very very Happy. Studied for 11 hrs :))))))))) YES :))))))</t>
+  </si>
+  <si>
+    <t>GAve reg expa test. Gave full syllabus test advanced 2. Received 83.85 marks. Best score till now</t>
+  </si>
+  <si>
+    <t>Very productive morning. At night I was feeling very low.</t>
   </si>
 </sst>
 </file>
@@ -3064,7 +3070,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B365" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C369" sqref="C369"/>
+      <selection activeCell="D371" sqref="D371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11423,6 +11429,21 @@
       </c>
       <c r="B371" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E371" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F371" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G371" s="24" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="372" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added 15th Nov 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34D0BC6-662F-4C9E-90F6-0E6F77B6E93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C04905-5666-4A3F-9450-E906AD9B3F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2169" uniqueCount="635">
   <si>
     <t>Date</t>
   </si>
@@ -2252,6 +2252,15 @@
   </si>
   <si>
     <t>65qs`</t>
+  </si>
+  <si>
+    <t>Couid not study in the morning. Very little study at night. Busy with project work</t>
+  </si>
+  <si>
+    <t>Bad day, unproductive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Went out for watching KANTARA movie. </t>
   </si>
 </sst>
 </file>
@@ -3075,8 +3084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B364" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G367" sqref="G367"/>
+    <sheetView tabSelected="1" topLeftCell="B366" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D373" sqref="D373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11459,6 +11468,21 @@
       <c r="B372" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C372" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E372" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="F372" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G372" s="12" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="373" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A373" s="10">
@@ -11466,6 +11490,9 @@
       </c>
       <c r="B373" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="374" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added 20th Nov 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7371038D-9350-4F1E-99D4-A225C5D392EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE60A24-F186-405D-9C20-55CCF93BD099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2188" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2196" uniqueCount="647">
   <si>
     <t>Date</t>
   </si>
@@ -2282,6 +2282,21 @@
   </si>
   <si>
     <t>Moderate day.</t>
+  </si>
+  <si>
+    <t>Studied algo for 2hrs. Completed till TOH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20pgs </t>
+  </si>
+  <si>
+    <t>Moderate Day.</t>
+  </si>
+  <si>
+    <t>Woke up at 6:40 am. Started studying from 7:15am</t>
+  </si>
+  <si>
+    <t>13pg</t>
   </si>
 </sst>
 </file>
@@ -3106,7 +3121,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B371" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C373" sqref="C373"/>
+      <selection activeCell="F378" sqref="F378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11604,6 +11619,21 @@
       <c r="B377" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C377" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="E377" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F377" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G377" s="1" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="378" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A378" s="10">
@@ -11611,6 +11641,15 @@
       </c>
       <c r="B378" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="D378" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="E378" s="11" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="379" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added TIFR CSE pdf
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F067CA94-9413-4C2F-B83F-242F078BBD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FFA442-5CF2-4D27-A9F0-EF36B3B2BBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -2293,13 +2293,13 @@
     <t>Moderate Day.</t>
   </si>
   <si>
-    <t>Woke up at 6:40 am. Started studying from 7:15am. Completed upto Master Theorem, merge sort, straight merge sort</t>
-  </si>
-  <si>
-    <t>38pgs</t>
-  </si>
-  <si>
-    <t>Good Going</t>
+    <t>Woke up at 6:40 am. Started studying from 7:15am. Completed upto Master Theorem, merge sort, straight merge sort, all merge sort qs (upto pg 294)</t>
+  </si>
+  <si>
+    <t>45pgs</t>
+  </si>
+  <si>
+    <t>Great Going</t>
   </si>
 </sst>
 </file>
@@ -3124,7 +3124,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B372" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E377" sqref="E377"/>
+      <selection activeCell="C379" sqref="C379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11652,7 +11652,7 @@
         <v>646</v>
       </c>
       <c r="E378" s="11" t="s">
-        <v>292</v>
+        <v>227</v>
       </c>
       <c r="F378" s="1" t="s">
         <v>352</v>

</xml_diff>

<commit_message>
Added 21st Nov 2022
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AC37CC-12FB-4DC0-9E3A-39C2AB3A25E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27430C2-7C93-43CC-B661-1FBFA8EEB27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2202" uniqueCount="649">
   <si>
     <t>Date</t>
   </si>
@@ -2300,6 +2300,9 @@
   </si>
   <si>
     <t>48pgs</t>
+  </si>
+  <si>
+    <t>Completed till Quick sort revision</t>
   </si>
 </sst>
 </file>
@@ -3124,7 +3127,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B372" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G378" sqref="G378"/>
+      <selection activeCell="G379" sqref="G379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11667,6 +11670,18 @@
       </c>
       <c r="B379" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="D379" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E379" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F379" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="380" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated sheet and solving pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2973C4-E0B2-4362-8440-2CD071C847F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778B7DC3-D4E8-4CD7-A2BA-2783F5FAA0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2263" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="666">
   <si>
     <t>Date</t>
   </si>
@@ -2348,6 +2348,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Studying Algo. Solving Pyqs -&gt; graph algorithms</t>
+  </si>
+  <si>
+    <t>3qs</t>
   </si>
 </sst>
 </file>
@@ -2633,7 +2639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2762,6 +2768,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="10" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3171,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B385" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E388" sqref="E388"/>
+    <sheetView tabSelected="1" topLeftCell="B392" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E398" sqref="E398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12015,6 +12024,21 @@
       <c r="B392" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C392" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E392" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F392" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G392" s="24" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="393" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A393" s="10">
@@ -12023,6 +12047,21 @@
       <c r="B393" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C393" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E393" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F393" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G393" s="24" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="394" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A394" s="10">
@@ -12031,6 +12070,21 @@
       <c r="B394" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C394" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="D394" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E394" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F394" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G394" s="24" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="395" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A395" s="10">
@@ -12039,6 +12093,21 @@
       <c r="B395" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C395" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="D395" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E395" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F395" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G395" s="24" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="396" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A396" s="10">
@@ -12047,6 +12116,19 @@
       <c r="B396" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C396" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="D396" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="E396" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="F396" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G396" s="44"/>
     </row>
     <row r="397" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A397" s="10">
@@ -12622,7 +12704,7 @@
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D379 D385:D1048576 E380:E384">
+  <conditionalFormatting sqref="D1:D379 E380:E384 D385:D1048576">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"10-40qs or pgs"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Completed 10qs on algo
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778B7DC3-D4E8-4CD7-A2BA-2783F5FAA0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664C683-D6EE-40AB-B084-BFD14038D05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -20,19 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="665">
   <si>
     <t>Date</t>
   </si>
@@ -2351,9 +2344,6 @@
   </si>
   <si>
     <t>Studying Algo. Solving Pyqs -&gt; graph algorithms</t>
-  </si>
-  <si>
-    <t>3qs</t>
   </si>
 </sst>
 </file>
@@ -2639,7 +2629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2768,9 +2758,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="10" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3181,7 +3168,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B392" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E398" sqref="E398"/>
+      <selection activeCell="G396" sqref="G396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12120,15 +12107,14 @@
         <v>664</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>665</v>
+        <v>322</v>
       </c>
       <c r="E396" s="11" t="s">
-        <v>394</v>
+        <v>650</v>
       </c>
       <c r="F396" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G396" s="44"/>
     </row>
     <row r="397" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A397" s="10">

</xml_diff>

<commit_message>
About to complete 1.6 in algo
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA9EB52-BD6A-472E-98CD-88D494E4D598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F421B5F-1A5C-4667-8B13-C6F59D98564F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="670">
   <si>
     <t>Date</t>
   </si>
@@ -2346,9 +2346,6 @@
     <t>Studying Algo. Solving Pyqs -&gt; graph algorithms</t>
   </si>
   <si>
-    <t>Semester has ended. Back at home. Full studies starts</t>
-  </si>
-  <si>
     <t>Came back from Kalyani to Siliguri. Could not study</t>
   </si>
   <si>
@@ -2356,6 +2353,12 @@
   </si>
   <si>
     <t>Moderate study</t>
+  </si>
+  <si>
+    <t>Semester has ended. Back at home. Full studies starts. Did algo pyqs at a stretch</t>
+  </si>
+  <si>
+    <t>Great study and great feeling/ About to complete 1.6 graph alogorithms</t>
   </si>
 </sst>
 </file>
@@ -3179,8 +3182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A393" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A399" sqref="A399"/>
+    <sheetView tabSelected="1" topLeftCell="B393" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C395" sqref="C395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12128,7 +12131,7 @@
         <v>352</v>
       </c>
       <c r="G396" s="24" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="397" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -12162,7 +12165,7 @@
         <v>6</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D398" s="1" t="s">
         <v>413</v>
@@ -12174,7 +12177,7 @@
         <v>413</v>
       </c>
       <c r="G398" s="12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="399" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -12185,7 +12188,19 @@
         <v>7</v>
       </c>
       <c r="C399" s="1" t="s">
-        <v>665</v>
+        <v>668</v>
+      </c>
+      <c r="D399" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E399" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="F399" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G399" s="33" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="400" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed till greed algos
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8CD972-AD98-4C2C-98B3-ED55B0DDFDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C961B3A-1E67-4D9D-A764-01934F23C8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -2361,7 +2361,7 @@
     <t>Great study and great feeling/ About to complete 1.6 graph alogorithms</t>
   </si>
   <si>
-    <t>Completed Graph Algorthims</t>
+    <t>Completed Graph Algorthims, graphsearch qs, greedy algo</t>
   </si>
 </sst>
 </file>
@@ -3186,7 +3186,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B393" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G400" sqref="G400"/>
+      <selection activeCell="H400" sqref="H400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12217,10 +12217,10 @@
         <v>670</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>336</v>
+        <v>379</v>
       </c>
       <c r="E400" s="11" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="F400" s="1" t="s">
         <v>352</v>

</xml_diff>

<commit_message>
Completed Huffman Coding, Hashing
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C961B3A-1E67-4D9D-A764-01934F23C8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E29F122-9EEC-4C0D-9108-03130A0F5223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="676">
   <si>
     <t>Date</t>
   </si>
@@ -2362,6 +2362,21 @@
   </si>
   <si>
     <t>Completed Graph Algorthims, graphsearch qs, greedy algo</t>
+  </si>
+  <si>
+    <t>Very  good study</t>
+  </si>
+  <si>
+    <t>Travelled to Balurghat due to Sister's marriage registry. No study in morning.</t>
+  </si>
+  <si>
+    <t>Completed Hashing, huffman coding</t>
+  </si>
+  <si>
+    <t>8qs</t>
+  </si>
+  <si>
+    <t>10min</t>
   </si>
 </sst>
 </file>
@@ -3185,8 +3200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B393" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H400" sqref="H400"/>
+    <sheetView tabSelected="1" topLeftCell="B395" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F402" sqref="F402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12225,24 +12240,54 @@
       <c r="F400" s="1" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="401" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G400" s="33" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A401" s="10">
         <v>44908</v>
       </c>
       <c r="B401" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="402" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C401" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D401" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E401" s="11" t="s">
+        <v>675</v>
+      </c>
+      <c r="F401" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G401" s="12" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A402" s="10">
         <v>44909</v>
       </c>
       <c r="B402" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="403" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C402" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="D402" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="E402" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="F402" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A403" s="10">
         <v>44910</v>
       </c>
@@ -12250,7 +12295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A404" s="10">
         <v>44911</v>
       </c>
@@ -12258,7 +12303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="405" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A405" s="10">
         <v>44912</v>
       </c>
@@ -12266,7 +12311,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="406" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A406" s="10">
         <v>44913</v>
       </c>
@@ -12274,7 +12319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A407" s="10">
         <v>44914</v>
       </c>
@@ -12282,7 +12327,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="408" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A408" s="10">
         <v>44915</v>
       </c>
@@ -12290,7 +12335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A409" s="10">
         <v>44916</v>
       </c>
@@ -12298,7 +12343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A410" s="10">
         <v>44917</v>
       </c>
@@ -12306,7 +12351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="411" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A411" s="10">
         <v>44918</v>
       </c>
@@ -12314,7 +12359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A412" s="10">
         <v>44919</v>
       </c>
@@ -12322,7 +12367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="413" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A413" s="10">
         <v>44920</v>
       </c>
@@ -12330,7 +12375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="414" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A414" s="10">
         <v>44921</v>
       </c>
@@ -12338,7 +12383,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="415" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A415" s="10">
         <v>44922</v>
       </c>
@@ -12346,7 +12391,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="416" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A416" s="10">
         <v>44923</v>
       </c>

</xml_diff>

<commit_message>
Completed 25 sorting pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDE2EE1-6756-4C6D-9C80-B5ACA0B4FC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58C6350-191F-4AF6-AF68-12A32A0AFBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -2403,7 +2403,7 @@
     <t>Less study</t>
   </si>
   <si>
-    <t>Sat to study at 11:15am. Completed recurrence qs, recursion, searching</t>
+    <t>Sat to study at 11:15am. Completed recurrence qs, recursion, searching, 24 sorting qs</t>
   </si>
 </sst>
 </file>
@@ -3228,7 +3228,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C408" sqref="C408"/>
+      <selection activeCell="F407" sqref="F407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12420,10 +12420,10 @@
         <v>684</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>322</v>
+        <v>340</v>
       </c>
       <c r="E407" s="11" t="s">
-        <v>277</v>
+        <v>226</v>
       </c>
     </row>
     <row r="408" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Gave GO Mock 2, updated sheet
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAC3052-F7D6-4FD9-9D40-07E8CB495391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3DE998-37E4-4D64-AB65-416B07806A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="688">
   <si>
     <t>Date</t>
   </si>
@@ -2410,6 +2410,9 @@
   </si>
   <si>
     <t xml:space="preserve">Great day. Full concentrated study. </t>
+  </si>
+  <si>
+    <t>Gave Go Classes Mock 2. Received 59.33 marks. Not happy, completed analysis. Studying great. Doing Algo PYQs</t>
   </si>
 </sst>
 </file>
@@ -3234,7 +3237,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G412" sqref="G412"/>
+      <selection activeCell="G408" sqref="G408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12444,6 +12447,18 @@
       </c>
       <c r="B408" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="E408" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="F408" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="409" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed 18qs of ST algo
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3DE998-37E4-4D64-AB65-416B07806A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD60E01-E327-491C-9559-98E88B70D09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="690">
   <si>
     <t>Date</t>
   </si>
@@ -2412,7 +2412,13 @@
     <t xml:space="preserve">Great day. Full concentrated study. </t>
   </si>
   <si>
-    <t>Gave Go Classes Mock 2. Received 59.33 marks. Not happy, completed analysis. Studying great. Doing Algo PYQs</t>
+    <t>13hrs</t>
+  </si>
+  <si>
+    <t>Gave Go Classes Mock 2. Received 59.33 marks. Not happy, completed analysis. Studying great. Doing Algo PYQs, 18 qs of spanning trees done</t>
+  </si>
+  <si>
+    <t>Awesome study</t>
   </si>
 </sst>
 </file>
@@ -3237,7 +3243,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G408" sqref="G408"/>
+      <selection activeCell="C410" sqref="C410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12449,16 +12455,19 @@
         <v>9</v>
       </c>
       <c r="C408" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E408" s="11" t="s">
         <v>687</v>
-      </c>
-      <c r="D408" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="E408" s="11" t="s">
-        <v>626</v>
       </c>
       <c r="F408" s="1" t="s">
         <v>400</v>
+      </c>
+      <c r="G408" s="33" t="s">
+        <v>689</v>
       </c>
     </row>
     <row r="409" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed Spanning trees in algo pyq
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD60E01-E327-491C-9559-98E88B70D09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3647DF54-0F5B-4B62-ACB2-C8D9018DC1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="691">
   <si>
     <t>Date</t>
   </si>
@@ -2419,6 +2419,9 @@
   </si>
   <si>
     <t>Awesome study</t>
+  </si>
+  <si>
+    <t>Completed Spanning trees q</t>
   </si>
 </sst>
 </file>
@@ -3243,7 +3246,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C410" sqref="C410"/>
+      <selection activeCell="E409" sqref="E409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12476,6 +12479,15 @@
       </c>
       <c r="B409" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D409" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E409" s="11" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="410" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated sheet, completed Algo
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3647DF54-0F5B-4B62-ACB2-C8D9018DC1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AF4BAA-E7F5-42DA-B4D2-AB0EE6963B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="692">
   <si>
     <t>Date</t>
   </si>
@@ -2421,7 +2421,10 @@
     <t>Awesome study</t>
   </si>
   <si>
-    <t>Completed Spanning trees q</t>
+    <t xml:space="preserve">Completed Spanning trees q. Completed Algo PYQS also. Studied 2 lectures of Countability by Deepak poonia Sir. </t>
+  </si>
+  <si>
+    <t>Great Day. Feeling Awesome</t>
   </si>
 </sst>
 </file>
@@ -3246,7 +3249,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E409" sqref="E409"/>
+      <selection activeCell="D413" sqref="D413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12484,10 +12487,16 @@
         <v>690</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>322</v>
+        <v>502</v>
       </c>
       <c r="E409" s="11" t="s">
-        <v>241</v>
+        <v>687</v>
+      </c>
+      <c r="F409" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G409" s="33" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="410" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Algo test 2 given
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D607C01-077D-4CD6-A2AE-3C7F7776159F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B0FD47-5198-4687-8CA4-A9640B91A1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2357" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="695">
   <si>
     <t>Date</t>
   </si>
@@ -2428,6 +2428,12 @@
   </si>
   <si>
     <t>Today Morning I gave Go classes Mock -3. Absolutely bad performance due to very careless mistakes and wasting time. I have analysed it half. At night started with CD. Today's day is going slow</t>
+  </si>
+  <si>
+    <t>Algo test 2 given. Analysis completed</t>
+  </si>
+  <si>
+    <t>17qs</t>
   </si>
 </sst>
 </file>
@@ -3252,7 +3258,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G410" sqref="G410"/>
+      <selection activeCell="E411" sqref="E411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12528,6 +12534,15 @@
       </c>
       <c r="B411" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="F411" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="412" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated sheet, started CD pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F140E3-088F-4D16-88BC-DA4ECD25D13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A4BE47-AC8D-4834-90B0-3921B576D927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2368" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="699">
   <si>
     <t>Date</t>
   </si>
@@ -2443,6 +2443,9 @@
   </si>
   <si>
     <t>Awesome study. Completed CD in 1 day</t>
+  </si>
+  <si>
+    <t>Started CD Pyqs</t>
   </si>
 </sst>
 </file>
@@ -3267,7 +3270,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C411" sqref="C411"/>
+      <selection activeCell="D413" sqref="D413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12592,6 +12595,9 @@
       </c>
       <c r="B413" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C413" s="1" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="414" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed CD Grammar pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD907A2-D3DF-4117-9B71-30F29590F540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C32C5D-2FDA-4C99-9873-7AF1A8797A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2377" uniqueCount="701">
   <si>
     <t>Date</t>
   </si>
@@ -2445,7 +2445,13 @@
     <t>Awesome study. Completed CD in 1 day</t>
   </si>
   <si>
-    <t>Started CD Pyqs, completed pyqs of AST, assembler</t>
+    <t>Completed 42pyqs of Grammar CD,</t>
+  </si>
+  <si>
+    <t>42qs</t>
+  </si>
+  <si>
+    <t>Started CD Pyqs, completed pyqs of AST, assembler, Code opti, comp phase,exp eval</t>
   </si>
 </sst>
 </file>
@@ -3269,8 +3275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C413" sqref="C413"/>
+    <sheetView tabSelected="1" topLeftCell="B407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H414" sqref="H414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12597,7 +12603,19 @@
         <v>7</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>698</v>
+        <v>700</v>
+      </c>
+      <c r="D413" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E413" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="F413" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G413" s="13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="414" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -12606,6 +12624,18 @@
       </c>
       <c r="B414" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="E414" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F414" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="415" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed PArameter passing pyqs
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6455E627-EB35-45FC-9D32-B625A7DD43BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBB0BA2-1872-4983-AA58-C87FBE8166FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="702">
   <si>
     <t>Date</t>
   </si>
@@ -2448,7 +2448,13 @@
     <t>Started CD Pyqs, completed pyqs of AST, assembler, Code opti, comp phase,exp eval</t>
   </si>
   <si>
-    <t>Completed 42pyqs of Grammar CD, icg, la. Also analysed Mock-3. Linker pyqs done</t>
+    <t>Completed  2.14 Parameter Passing (14)</t>
+  </si>
+  <si>
+    <t>Completed 42pyqs of Grammar CD, icg, la. Also analysed Mock-3. Linker pyqs, 2.12 Lr Parsing (2), 2.13 Macros (4), done</t>
+  </si>
+  <si>
+    <t>Great day. Very productive</t>
   </si>
 </sst>
 </file>
@@ -3272,8 +3278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B407" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E414" sqref="E414"/>
+    <sheetView tabSelected="1" topLeftCell="B414" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E417" sqref="E417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12623,16 +12629,19 @@
         <v>8</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="D414" s="1">
-        <v>63</v>
+        <v>700</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>577</v>
       </c>
       <c r="E414" s="11" t="s">
-        <v>226</v>
+        <v>380</v>
       </c>
       <c r="F414" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="G414" s="33" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="415" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -12641,6 +12650,15 @@
       </c>
       <c r="B415" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E415" s="11" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="416" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Parsing (46) pyqs done
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBB0BA2-1872-4983-AA58-C87FBE8166FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67B7382-9B8F-4BDE-9FF2-444EB5C2B208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -2448,13 +2448,13 @@
     <t>Started CD Pyqs, completed pyqs of AST, assembler, Code opti, comp phase,exp eval</t>
   </si>
   <si>
-    <t>Completed  2.14 Parameter Passing (14)</t>
-  </si>
-  <si>
     <t>Completed 42pyqs of Grammar CD, icg, la. Also analysed Mock-3. Linker pyqs, 2.12 Lr Parsing (2), 2.13 Macros (4), done</t>
   </si>
   <si>
     <t>Great day. Very productive</t>
+  </si>
+  <si>
+    <t>Completed  2.14 Parameter Passing (14),  Parsing (46)</t>
   </si>
 </sst>
 </file>
@@ -3279,7 +3279,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B414" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E417" sqref="E417"/>
+      <selection activeCell="F415" sqref="F415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12629,7 +12629,7 @@
         <v>8</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D414" s="1" t="s">
         <v>577</v>
@@ -12641,7 +12641,7 @@
         <v>352</v>
       </c>
       <c r="G414" s="33" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="415" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -12652,13 +12652,13 @@
         <v>9</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>323</v>
+        <v>443</v>
       </c>
       <c r="E415" s="11" t="s">
-        <v>650</v>
+        <v>360</v>
       </c>
     </row>
     <row r="416" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Plenty of CD py1s 82pyqs done.
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67B7382-9B8F-4BDE-9FF2-444EB5C2B208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E12B4ED-DCC2-4571-8E79-FDC5CD7551D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="703">
   <si>
     <t>Date</t>
   </si>
@@ -2454,7 +2454,12 @@
     <t>Great day. Very productive</t>
   </si>
   <si>
-    <t>Completed  2.14 Parameter Passing (14),  Parsing (46)</t>
+    <t>Completed  2.14 Parameter Passing (14),  Parsing (46),  Static Single Assignment (2), Register Allocation (2), 
+Syntax Directed Translation (11) , 2.20 Target Code Generation (4), 2.21 Variable Scope (2), 
+2.22 Viable Prefix (1)</t>
+  </si>
+  <si>
+    <t>82qs</t>
   </si>
 </sst>
 </file>
@@ -3279,7 +3284,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B414" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F415" sqref="F415"/>
+      <selection activeCell="G415" sqref="G415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12655,10 +12660,16 @@
         <v>701</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="E415" s="11" t="s">
-        <v>360</v>
+        <v>202</v>
+      </c>
+      <c r="F415" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G415" s="33" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="416" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated my test tracker
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60452D1-AC9E-428D-B2EB-E77FE549FDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979EE230-9FC1-4426-895C-CCD3640F1AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2386" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2387" uniqueCount="704">
   <si>
     <t>Date</t>
   </si>
@@ -2462,10 +2462,7 @@
     <t>82qs</t>
   </si>
   <si>
-    <t>Completed CD revision as well as all pyqs done.</t>
-  </si>
-  <si>
-    <t>19qs</t>
+    <t>Completed CD revision as well as all pyqs done. Gave GO Classes CD-1,2,3 tests, with analysis done</t>
   </si>
 </sst>
 </file>
@@ -3290,7 +3287,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B414" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D417" sqref="D417"/>
+      <selection activeCell="G416" sqref="G416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12689,10 +12686,13 @@
         <v>703</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>704</v>
+        <v>480</v>
       </c>
       <c r="E416" s="11" t="s">
-        <v>277</v>
+        <v>226</v>
+      </c>
+      <c r="F416" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Mock-4 Go Classes Marks
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979EE230-9FC1-4426-895C-CCD3640F1AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CAB155-6783-4D86-9B5D-7D7D623F4BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2387" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2391" uniqueCount="706">
   <si>
     <t>Date</t>
   </si>
@@ -2462,14 +2462,32 @@
     <t>82qs</t>
   </si>
   <si>
-    <t>Completed CD revision as well as all pyqs done. Gave GO Classes CD-1,2,3 tests, with analysis done</t>
+    <r>
+      <t>Completed CD revision as well as all pyqs done. Gave GO Classes CD-1,2,3 tests, with analysis done. Gave 2 CD Subject tests from Gate Overflow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Got Rank 1 in both.</t>
+    </r>
+  </si>
+  <si>
+    <t>Great day. Very productive and good results in CD prep.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woke up late. Started the last subject -&gt; DL revision. Completed Logic functions. Watched vids in functional completeness from GO Classes </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2544,6 +2562,13 @@
     <font>
       <sz val="36"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3287,7 +3312,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B414" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G416" sqref="G416"/>
+      <selection activeCell="F417" sqref="F417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12686,24 +12711,36 @@
         <v>703</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="E416" s="11" t="s">
-        <v>226</v>
+        <v>626</v>
       </c>
       <c r="F416" s="1" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="417" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G416" s="33" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A417" s="10">
         <v>44924</v>
       </c>
       <c r="B417" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="418" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C417" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E417" s="11" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A418" s="10">
         <v>44925</v>
       </c>
@@ -12711,7 +12748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A419" s="10">
         <v>44926</v>
       </c>
@@ -12719,7 +12756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="420" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A420" s="10">
         <v>44927</v>
       </c>
@@ -12727,7 +12764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="421" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A421" s="10">
         <v>44928</v>
       </c>
@@ -12735,7 +12772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="422" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A422" s="10">
         <v>44929</v>
       </c>
@@ -12743,7 +12780,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="423" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A423" s="10">
         <v>44930</v>
       </c>
@@ -12751,7 +12788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="424" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A424" s="10">
         <v>44931</v>
       </c>
@@ -12759,7 +12796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="425" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A425" s="10">
         <v>44932</v>
       </c>
@@ -12767,7 +12804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="426" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A426" s="10">
         <v>44933</v>
       </c>
@@ -12775,7 +12812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="427" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A427" s="10">
         <v>44934</v>
       </c>
@@ -12783,7 +12820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="428" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A428" s="10">
         <v>44935</v>
       </c>
@@ -12791,7 +12828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="429" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A429" s="10">
         <v>44936</v>
       </c>
@@ -12799,7 +12836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="430" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A430" s="10">
         <v>44937</v>
       </c>
@@ -12807,7 +12844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A431" s="10">
         <v>44938</v>
       </c>
@@ -12815,7 +12852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A432" s="10">
         <v>44939</v>
       </c>

</xml_diff>

<commit_message>
Cuurently in minm no of gates topic of DL PYQ
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7057B738-A142-42F8-8696-92A96B83F6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5599230C-4FF6-437B-A88E-7B1DCEFB7E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="718">
   <si>
     <t>Date</t>
   </si>
@@ -2510,10 +2510,13 @@
     <t>Solving DL pyqs. Now in circuit output</t>
   </si>
   <si>
-    <t>Completed upo Decoder Pyqs</t>
-  </si>
-  <si>
-    <t>50pyqs</t>
+    <t>Completed upto Decoder Pyqs flip flops done. Gave 2021 set -2 paper. Received Normalised Marks = 61.5. Rank =270</t>
+  </si>
+  <si>
+    <t>50pyqs + 65qs</t>
+  </si>
+  <si>
+    <t>Gave Test + Did Pyqs.</t>
   </si>
 </sst>
 </file>
@@ -3345,7 +3348,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B417" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E419" sqref="E419"/>
+      <selection activeCell="B424" sqref="B424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12908,10 +12911,13 @@
         <v>716</v>
       </c>
       <c r="E423" s="11" t="s">
-        <v>650</v>
+        <v>203</v>
       </c>
       <c r="F423" s="1" t="s">
-        <v>352</v>
+        <v>400</v>
+      </c>
+      <c r="G423" s="1" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="424" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Finally completed DL along with PYQS
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5599230C-4FF6-437B-A88E-7B1DCEFB7E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A561F9F8-AE63-46DE-9005-0B49E1A06B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="722">
   <si>
     <t>Date</t>
   </si>
@@ -2517,6 +2517,18 @@
   </si>
   <si>
     <t>Gave Test + Did Pyqs.</t>
+  </si>
+  <si>
+    <t>Completed all DL PYQS . Took a lot of time to do all 300 qs. Feeling Great</t>
+  </si>
+  <si>
+    <t>Did DL Pyqs</t>
+  </si>
+  <si>
+    <t>80qs</t>
+  </si>
+  <si>
+    <t>Good day. Still DL not completed</t>
   </si>
 </sst>
 </file>
@@ -3347,8 +3359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B417" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B424" sqref="B424"/>
+    <sheetView tabSelected="1" topLeftCell="B419" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F425" sqref="F425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12927,6 +12939,21 @@
       <c r="B424" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C424" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="D424" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="E424" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="F424" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G424" s="1" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="425" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A425" s="10">
@@ -12934,6 +12961,15 @@
       </c>
       <c r="B425" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="D425" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="E425" s="11" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="426" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Made final plan for GATE 2023
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A561F9F8-AE63-46DE-9005-0B49E1A06B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8F700-D628-499C-AF85-226EF9F69D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2433" uniqueCount="723">
   <si>
     <t>Date</t>
   </si>
@@ -2529,6 +2529,9 @@
   </si>
   <si>
     <t>Good day. Still DL not completed</t>
+  </si>
+  <si>
+    <t>GREAT DAY</t>
   </si>
 </sst>
 </file>
@@ -3360,7 +3363,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B419" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F425" sqref="F425"/>
+      <selection activeCell="D423" sqref="D423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12928,7 +12931,7 @@
       <c r="F423" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="G423" s="1" t="s">
+      <c r="G423" s="33" t="s">
         <v>717</v>
       </c>
     </row>
@@ -12951,7 +12954,7 @@
       <c r="F424" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G424" s="1" t="s">
+      <c r="G424" s="33" t="s">
         <v>721</v>
       </c>
     </row>
@@ -12970,6 +12973,12 @@
       </c>
       <c r="E425" s="11" t="s">
         <v>203</v>
+      </c>
+      <c r="F425" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G425" s="33" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="426" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
analysed go mock 2
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A08EDA-8042-402D-AA88-E84B243DAB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABA3B54-A255-4898-8572-C68D1178FAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="730">
   <si>
     <t>Date</t>
   </si>
@@ -2538,6 +2538,21 @@
   </si>
   <si>
     <t>Great day. Made plans</t>
+  </si>
+  <si>
+    <t>Gave AIMT of goclasses. Got only 44.33 marks. Rank 105/600</t>
+  </si>
+  <si>
+    <t>No a great day</t>
+  </si>
+  <si>
+    <t>Analysed yesterday's test. Revised dbms er model a little</t>
+  </si>
+  <si>
+    <t>10ogs</t>
+  </si>
+  <si>
+    <t>Not very productive,. Bbut learnt a lot</t>
   </si>
 </sst>
 </file>
@@ -3368,8 +3383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B420" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C423" sqref="C423"/>
+    <sheetView tabSelected="1" topLeftCell="B422" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G426" sqref="G426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13017,6 +13032,21 @@
       <c r="B427" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C427" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E427" s="11" t="s">
+        <v>650</v>
+      </c>
+      <c r="F427" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G427" s="12" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="428" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A428" s="10">
@@ -13024,6 +13054,21 @@
       </c>
       <c r="B428" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D428" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="E428" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="F428" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G428" s="13" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="429" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed analysing GO MOCK -2
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABA3B54-A255-4898-8572-C68D1178FAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217C1BB2-73FA-4D78-9D18-60279D503800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="732">
   <si>
     <t>Date</t>
   </si>
@@ -2553,6 +2553,12 @@
   </si>
   <si>
     <t>Not very productive,. Bbut learnt a lot</t>
+  </si>
+  <si>
+    <t>Completed analysis of MOCK 2 of GO</t>
+  </si>
+  <si>
+    <t>Not very good marks = 52.33. Difficult paper but wasted time in few qs</t>
   </si>
 </sst>
 </file>
@@ -3384,7 +3390,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B422" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G426" sqref="G426"/>
+      <selection activeCell="C426" sqref="C426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13077,6 +13083,21 @@
       </c>
       <c r="B429" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="D429" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E429" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="F429" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G429" s="33" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="430" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated sheet 11th jan 2023
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217C1BB2-73FA-4D78-9D18-60279D503800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65413A92-B860-47D1-B363-4C1B518BCB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="733">
   <si>
     <t>Date</t>
   </si>
@@ -2559,6 +2559,9 @@
   </si>
   <si>
     <t>Not very good marks = 52.33. Difficult paper but wasted time in few qs</t>
+  </si>
+  <si>
+    <t>Gave MADE EASY GATE MOCK 1. GOT 64.33. Rank 8/107. Satisfied although made 18 incorrect.</t>
   </si>
 </sst>
 </file>
@@ -3389,8 +3392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B422" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C426" sqref="C426"/>
+    <sheetView tabSelected="1" topLeftCell="A423" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E430" sqref="E430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13106,6 +13109,12 @@
       </c>
       <c r="B430" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="C430" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="D430" s="1" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="431" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Made ChatGPT create my routine for the upcoming days
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65413A92-B860-47D1-B363-4C1B518BCB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281DF434-FCFA-4F92-9B40-CA907DCEF5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="738">
   <si>
     <t>Date</t>
   </si>
@@ -2562,6 +2562,21 @@
   </si>
   <si>
     <t>Gave MADE EASY GATE MOCK 1. GOT 64.33. Rank 8/107. Satisfied although made 18 incorrect.</t>
+  </si>
+  <si>
+    <t>Analysing go mock2. Going through unattemted topics</t>
+  </si>
+  <si>
+    <t>40+pgs</t>
+  </si>
+  <si>
+    <t>Going good</t>
+  </si>
+  <si>
+    <t>Could have utilised it better</t>
+  </si>
+  <si>
+    <t>Revised the following topics: endianness, Isolated, Mem-mapped IO, multilevel cache</t>
   </si>
 </sst>
 </file>
@@ -3392,8 +3407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A423" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E430" sqref="E430"/>
+    <sheetView tabSelected="1" topLeftCell="B429" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C433" sqref="C433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13116,6 +13131,15 @@
       <c r="D430" s="1" t="s">
         <v>480</v>
       </c>
+      <c r="E430" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F430" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G430" s="33" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="431" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A431" s="10">
@@ -13124,6 +13148,21 @@
       <c r="B431" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C431" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="D431" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="E431" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="F431" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="G431" s="24" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="432" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A432" s="10">
@@ -13131,6 +13170,9 @@
       </c>
       <c r="B432" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Gave tests and made chatgpt to make a routine
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281DF434-FCFA-4F92-9B40-CA907DCEF5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D276E469-A14F-49AD-A827-42A2296E7EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="740">
   <si>
     <t>Date</t>
   </si>
@@ -2576,7 +2576,18 @@
     <t>Could have utilised it better</t>
   </si>
   <si>
-    <t>Revised the following topics: endianness, Isolated, Mem-mapped IO, multilevel cache</t>
+    <t>3.5hr</t>
+  </si>
+  <si>
+    <t>Revised the following topics: endianness, Isolated, Mem-mapped IO, multilevel cache. Gave COA test on cache. Got great marks</t>
+  </si>
+  <si>
+    <t>Today's plan is : 14th Jan:
+9:15am - 12:15pm: Weak in memory management chapter of OS
+12:15pm - 3:15pm: Weak in TCP, IP, and certain other parts of CN
+3:15pm - 6:15pm: Weak in normalization, transaction, SQL, relational algebra of DBMS
+6:15pm - 9:15pm: Test on Weak in memory management chapter of OS
+9:15pm - 1:00am: Test on Weak in TCP, IP, and certain other parts of CN. Gave TOC decidability test. Good marks received</t>
   </si>
 </sst>
 </file>
@@ -3407,8 +3418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B429" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C433" sqref="C433"/>
+    <sheetView tabSelected="1" topLeftCell="B430" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D433" sqref="D433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13172,18 +13183,39 @@
         <v>12</v>
       </c>
       <c r="C432" s="1" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="433" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>738</v>
+      </c>
+      <c r="D432" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E432" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="F432" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G432" s="13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A433" s="10">
         <v>44940</v>
       </c>
       <c r="B433" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="434" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C433" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="E433" s="11" t="s">
+        <v>737</v>
+      </c>
+      <c r="F433" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A434" s="10">
         <v>44941</v>
       </c>
@@ -13191,7 +13223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="435" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A435" s="10">
         <v>44942</v>
       </c>
@@ -13199,7 +13231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="436" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A436" s="10">
         <v>44943</v>
       </c>
@@ -13207,7 +13239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="437" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A437" s="10">
         <v>44944</v>
       </c>
@@ -13215,7 +13247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="438" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A438" s="10">
         <v>44945</v>
       </c>
@@ -13223,7 +13255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A439" s="10">
         <v>44946</v>
       </c>
@@ -13231,7 +13263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A440" s="10">
         <v>44947</v>
       </c>
@@ -13239,7 +13271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="441" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A441" s="10">
         <v>44948</v>
       </c>
@@ -13247,7 +13279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="442" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A442" s="10">
         <v>44949</v>
       </c>
@@ -13255,7 +13287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="443" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A443" s="10">
         <v>44950</v>
       </c>
@@ -13263,7 +13295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="444" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A444" s="10">
         <v>44951</v>
       </c>
@@ -13271,7 +13303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="445" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A445" s="10">
         <v>44952</v>
       </c>
@@ -13279,7 +13311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="446" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A446" s="10">
         <v>44953</v>
       </c>
@@ -13287,7 +13319,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="447" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A447" s="10">
         <v>44954</v>
       </c>
@@ -13295,7 +13327,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A448" s="10">
         <v>44955</v>
       </c>

</xml_diff>

<commit_message>
Added MADE EASY MOCK - 2 Marks
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10203AE8-979B-4275-A1AB-54275E5FB69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE83CD15-6153-4125-82F6-C7541D304085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="752">
   <si>
     <t>Date</t>
   </si>
@@ -2620,9 +2620,6 @@
     <t>Studied only in the morning.</t>
   </si>
   <si>
-    <t>Completed Mock-3 of go classes analysis</t>
-  </si>
-  <si>
     <t xml:space="preserve">Completed all analysis of every q of MOCK - 2 of GO CLASSES. It took many days tbh, but it was all worth it! Started with Mock -3 </t>
   </si>
   <si>
@@ -2632,7 +2629,10 @@
     <t>65QS</t>
   </si>
   <si>
-    <t>8HRS</t>
+    <t>Gave MADE EASY GATE MOCK -2. GOT 65.02. Rank - 33/350</t>
+  </si>
+  <si>
+    <t>Completed Mock-3 of go classes analysis. Started Mock -4 analuysis</t>
   </si>
 </sst>
 </file>
@@ -3463,8 +3463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B433" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F438" sqref="F438"/>
+    <sheetView tabSelected="1" topLeftCell="B435" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G439" sqref="G439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13343,7 +13343,7 @@
         <v>10</v>
       </c>
       <c r="C437" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D437" s="1" t="s">
         <v>340</v>
@@ -13355,7 +13355,7 @@
         <v>352</v>
       </c>
       <c r="G437" s="33" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="438" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -13366,13 +13366,19 @@
         <v>11</v>
       </c>
       <c r="C438" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E438" s="11" t="s">
-        <v>751</v>
+        <v>571</v>
+      </c>
+      <c r="F438" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G438" s="33" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="439" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -13381,6 +13387,18 @@
       </c>
       <c r="B439" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="D439" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="E439" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F439" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="440" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Mock - 4 analysis done
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE83CD15-6153-4125-82F6-C7541D304085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A267F238-DEC2-41D2-A01A-F69CB9350CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2507" uniqueCount="754">
   <si>
     <t>Date</t>
   </si>
@@ -2633,6 +2633,12 @@
   </si>
   <si>
     <t>Completed Mock-3 of go classes analysis. Started Mock -4 analuysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed MOCk - 4 analysis </t>
+  </si>
+  <si>
+    <t>Good day</t>
   </si>
 </sst>
 </file>
@@ -3464,7 +3470,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B435" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G439" sqref="G439"/>
+      <selection activeCell="C438" sqref="C438"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13400,6 +13406,9 @@
       <c r="F439" s="1" t="s">
         <v>400</v>
       </c>
+      <c r="G439" s="33" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="440" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A440" s="10">
@@ -13407,6 +13416,18 @@
       </c>
       <c r="B440" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D440" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E440" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="F440" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="441" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Doing COA pyqs. 2nd time
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A267F238-DEC2-41D2-A01A-F69CB9350CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A795EA2-D437-49C8-8C94-91C10AE68645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2507" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="758">
   <si>
     <t>Date</t>
   </si>
@@ -2639,6 +2639,18 @@
   </si>
   <si>
     <t>Good day</t>
+  </si>
+  <si>
+    <t>Gave AIMT 2. Analysing.</t>
+  </si>
+  <si>
+    <t>Started doing PYQs for the 2nd time. Yes, I'm getting confidence :) Started with COA today</t>
+  </si>
+  <si>
+    <t>69qs</t>
+  </si>
+  <si>
+    <t>These days are going good,</t>
   </si>
 </sst>
 </file>
@@ -3469,8 +3481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B435" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C438" sqref="C438"/>
+    <sheetView tabSelected="1" topLeftCell="B436" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G442" sqref="G442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13429,6 +13441,9 @@
       <c r="F440" s="1" t="s">
         <v>352</v>
       </c>
+      <c r="G440" s="33" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="441" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A441" s="10">
@@ -13437,6 +13452,21 @@
       <c r="B441" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C441" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D441" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E441" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="F441" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G441" s="33" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="442" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A442" s="10">
@@ -13444,6 +13474,18 @@
       </c>
       <c r="B442" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C442" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D442" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="E442" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="F442" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="443" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Did COA, DBMS, DM
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A795EA2-D437-49C8-8C94-91C10AE68645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C91E25B-F709-4552-83CB-A038CD03A54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2523" uniqueCount="761">
   <si>
     <t>Date</t>
   </si>
@@ -2647,10 +2647,19 @@
     <t>Started doing PYQs for the 2nd time. Yes, I'm getting confidence :) Started with COA today</t>
   </si>
   <si>
-    <t>69qs</t>
-  </si>
-  <si>
     <t>These days are going good,</t>
+  </si>
+  <si>
+    <t>85qs</t>
+  </si>
+  <si>
+    <t>Great day.</t>
+  </si>
+  <si>
+    <t>Have been doing COA pyqs. P{ipeline left. Now switched to DBMS. Completed SQL. Then studied DM Graph theory. 99.9% done</t>
+  </si>
+  <si>
+    <t>Excellent Day</t>
   </si>
 </sst>
 </file>
@@ -3481,8 +3490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B436" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G442" sqref="G442"/>
+    <sheetView tabSelected="1" topLeftCell="B443" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D447" sqref="D447"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13442,7 +13451,7 @@
         <v>352</v>
       </c>
       <c r="G440" s="33" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="441" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -13465,7 +13474,7 @@
         <v>400</v>
       </c>
       <c r="G441" s="33" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="442" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -13479,13 +13488,16 @@
         <v>755</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="E442" s="11" t="s">
-        <v>626</v>
+        <v>687</v>
       </c>
       <c r="F442" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="G442" s="33" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="443" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -13494,6 +13506,21 @@
       </c>
       <c r="B443" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C443" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="D443" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E443" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="F443" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G443" s="33" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="444" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Studying, Revising, Pyqing OS
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C91E25B-F709-4552-83CB-A038CD03A54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E1E7ED-3EAB-4615-A959-AB5B82F07791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2523" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2527" uniqueCount="763">
   <si>
     <t>Date</t>
   </si>
@@ -2660,6 +2660,12 @@
   </si>
   <si>
     <t>Excellent Day</t>
+  </si>
+  <si>
+    <t>Today I took up OS. Revised every part very nicely. Noticed that I had not done process synch pyqs. Thus doiing them at night.</t>
+  </si>
+  <si>
+    <t>160pgs, 70qs</t>
   </si>
 </sst>
 </file>
@@ -3491,7 +3497,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B443" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D447" sqref="D447"/>
+      <selection activeCell="H444" sqref="H444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13529,6 +13535,18 @@
       </c>
       <c r="B444" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="C444" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="D444" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="E444" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="F444" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="445" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated everything before D-day
</commit_message>
<xml_diff>
--- a/My Entire Preparation Routine.xlsx
+++ b/My Entire Preparation Routine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D111C0C-3FED-40E9-95E6-1F45D0194FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1579FC-131A-424A-B742-63612D51B00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18287A40-332A-4038-84C1-F23C7058B3E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2550" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2573" uniqueCount="778">
   <si>
     <t>Date</t>
   </si>
@@ -2690,6 +2690,27 @@
   </si>
   <si>
     <t>Studied file allocation,. Revised COA pipeline completely. From today I will study all subject main notes till 1st Feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algo revision completed final time. </t>
+  </si>
+  <si>
+    <t>400pgs</t>
+  </si>
+  <si>
+    <t>Revising ALGO. Test by Bikram -1 . Completed within 1.5hrs whole paper 61qs.</t>
+  </si>
+  <si>
+    <t>Preparing for End game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revised all subjects from short notes in 1 day. I will definitely give my best tomorrow. </t>
+  </si>
+  <si>
+    <t>infinity</t>
+  </si>
+  <si>
+    <t>BEST DAY</t>
   </si>
 </sst>
 </file>
@@ -3510,7 +3531,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3520,8 +3541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F4770D-944A-4DB9-BEB9-6A754A07CC2A}">
   <dimension ref="A1:G463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B442" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E449" sqref="E449"/>
+    <sheetView tabSelected="1" topLeftCell="B447" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C450" sqref="C450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13668,7 +13689,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="449" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A449" s="10">
         <v>44956</v>
       </c>
@@ -13681,40 +13702,109 @@
       <c r="D449" s="1" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="450" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E449" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F449" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G449" s="33" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="450" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A450" s="10">
         <v>44957</v>
       </c>
       <c r="B450" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="451" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C450" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="D450" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="E450" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F450" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G450" s="33" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="451" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A451" s="10">
         <v>44958</v>
       </c>
       <c r="B451" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="452" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C451" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="D451" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="E451" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F451" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G451" s="33" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="452" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A452" s="10">
         <v>44959</v>
       </c>
       <c r="B452" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="453" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C452" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D452" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="E452" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="F452" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G452" s="33" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A453" s="10">
         <v>44960</v>
       </c>
       <c r="B453" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="454" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C453" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="D453" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="E453" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F453" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G453" s="33" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A454" s="10">
         <v>44961</v>
       </c>
@@ -13722,7 +13812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="455" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A455" s="10">
         <v>44962</v>
       </c>
@@ -13730,7 +13820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="456" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A456" s="10">
         <v>44963</v>
       </c>
@@ -13738,7 +13828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="457" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A457" s="10">
         <v>44964</v>
       </c>
@@ -13746,7 +13836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="458" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A458" s="10">
         <v>44965</v>
       </c>
@@ -13754,7 +13844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="459" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A459" s="10">
         <v>44966</v>
       </c>
@@ -13762,7 +13852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="460" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A460" s="10">
         <v>44967</v>
       </c>
@@ -13770,7 +13860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="461" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A461" s="10">
         <v>44968</v>
       </c>
@@ -13778,7 +13868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="462" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A462" s="10">
         <v>44969</v>
       </c>
@@ -13786,7 +13876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="463" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A463" s="10">
         <v>44970</v>
       </c>

</xml_diff>